<commit_message>
Teminando criacao da planilha
</commit_message>
<xml_diff>
--- a/dataFile.xlsx
+++ b/dataFile.xlsx
@@ -6,6 +6,7 @@
     <sheet name="list" sheetId="1" r:id="rId1"/>
     <sheet name="good" sheetId="2" r:id="rId2"/>
     <sheet name="bad" sheetId="3" r:id="rId3"/>
+    <sheet name="virustotal" sheetId="4" r:id="rId4"/>
   </sheets>
 </workbook>
 </file>
@@ -377,7 +378,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A60"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -392,307 +393,17 @@
         <v>38.143.66.142</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3">
-        <v>10152176195</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="str">
-        <v>46.29.10.30</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="str">
-        <v>165.22.219.222</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="str">
-        <v>185.81.68.21</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="str">
-        <v>114.139.46.250</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8">
-        <v>192241205251</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="str">
-        <v>51.195.47.176</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="str">
-        <v>161.97.160.249</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="str">
-        <v>192.24.192.231</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="str">
-        <v>49.232.218.12</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="str">
-        <v>107.189.12.34</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="str">
-        <v>185.200.118.90</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15">
-        <v>192241219154</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16">
-        <v>192241206202</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="str">
-        <v>185.54.230.73</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="str">
-        <v>176.58.107.136</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="str">
-        <v>80.82.70.228</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="str">
-        <v>46.101.76.96</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="str">
-        <v>43.153.67.197</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="str">
-        <v>202.4.117.45</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="str">
-        <v>188.166.75.56</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24">
-        <v>192241215252</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="str">
-        <v>185.122.204.39</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="str">
-        <v>103.119.144.59</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="str">
-        <v>192.241.216.62</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="str">
-        <v>158.255.7.157</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="str">
-        <v>45.61.186.4</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30">
-        <v>183245151169</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="str">
-        <v>206.189.25.255</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="str">
-        <v>200.73.130.31</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" t="str">
-        <v>164.88.86.170</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" t="str">
-        <v>139.162.77.84</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" t="str">
-        <v>192.227.134.78</v>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" t="str">
-        <v>51.89.41.120</v>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37">
-        <v>89248163158</v>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" t="str">
-        <v>43.153.71.131</v>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" t="str">
-        <v>95.154.29.197</v>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" t="str">
-        <v>192.241.213.58</v>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" t="str">
-        <v>108.156.60.17</v>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" t="str">
-        <v>175.24.124.152</v>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" t="str">
-        <v>92.255.85.239</v>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" t="str">
-        <v>159.65.192.80</v>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" t="str">
-        <v>205.164.107.52</v>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46">
-        <v>45141151243</v>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" t="str">
-        <v>192.241.206.47</v>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" t="str">
-        <v>192.241.200.47</v>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" t="str">
-        <v>145.239.198.34</v>
-      </c>
-    </row>
-    <row r="50">
-      <c r="A50">
-        <v>192241221102</v>
-      </c>
-    </row>
-    <row r="51">
-      <c r="A51">
-        <v>192241202204</v>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52" t="str">
-        <v>198.199.96.218</v>
-      </c>
-    </row>
-    <row r="53">
-      <c r="A53" t="str">
-        <v>139.99.62.61</v>
-      </c>
-    </row>
-    <row r="54">
-      <c r="A54" t="str">
-        <v>159.65.51.33</v>
-      </c>
-    </row>
-    <row r="55">
-      <c r="A55" t="str">
-        <v>192.241.209.7</v>
-      </c>
-    </row>
-    <row r="56">
-      <c r="A56" t="str">
-        <v>137.184.10.101</v>
-      </c>
-    </row>
-    <row r="57">
-      <c r="A57" t="str">
-        <v>45.95.55.230</v>
-      </c>
-    </row>
-    <row r="58">
-      <c r="A58" t="str">
-        <v>185.200.116.90</v>
-      </c>
-    </row>
-    <row r="59">
-      <c r="A59" t="str">
-        <v>10.136.50.26</v>
-      </c>
-    </row>
-    <row r="60">
-      <c r="A60" t="str">
-        <v>10.30.184.116</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:A60"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:A2"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:D40"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -716,8 +427,8 @@
         <v>38.143.66.142</v>
       </c>
       <c r="B2" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-GlobalTeleHost Corp.
+        <v xml:space="preserve">_x000d_
+GlobalTeleHost Corp._x000d_
 </v>
       </c>
       <c r="C2" t="str">
@@ -732,8 +443,8 @@
         <v>108.156.60.17</v>
       </c>
       <c r="B3" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-Amazon.com Inc.
+        <v xml:space="preserve">_x000d_
+Amazon.com Inc._x000d_
 </v>
       </c>
       <c r="C3" t="str">
@@ -748,8 +459,8 @@
         <v>38.143.66.142</v>
       </c>
       <c r="B4" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-GlobalTeleHost Corp.
+        <v xml:space="preserve">_x000d_
+GlobalTeleHost Corp._x000d_
 </v>
       </c>
       <c r="C4" t="str">
@@ -764,8 +475,8 @@
         <v>108.156.60.17</v>
       </c>
       <c r="B5" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-Amazon.com Inc.
+        <v xml:space="preserve">_x000d_
+Amazon.com Inc._x000d_
 </v>
       </c>
       <c r="C5" t="str">
@@ -780,8 +491,8 @@
         <v>38.143.66.142</v>
       </c>
       <c r="B6" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-GlobalTeleHost Corp.
+        <v xml:space="preserve">_x000d_
+GlobalTeleHost Corp._x000d_
 </v>
       </c>
       <c r="C6" t="str">
@@ -796,8 +507,8 @@
         <v>108.156.60.17</v>
       </c>
       <c r="B7" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-Amazon.com Inc.
+        <v xml:space="preserve">_x000d_
+Amazon.com Inc._x000d_
 </v>
       </c>
       <c r="C7" t="str">
@@ -812,8 +523,8 @@
         <v>38.143.66.142</v>
       </c>
       <c r="B8" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-GlobalTeleHost Corp.
+        <v xml:space="preserve">_x000d_
+GlobalTeleHost Corp._x000d_
 </v>
       </c>
       <c r="C8" t="str">
@@ -828,8 +539,8 @@
         <v>38.143.66.142</v>
       </c>
       <c r="B9" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-GlobalTeleHost Corp.
+        <v xml:space="preserve">_x000d_
+GlobalTeleHost Corp._x000d_
 </v>
       </c>
       <c r="C9" t="str">
@@ -844,8 +555,8 @@
         <v>38.143.66.142</v>
       </c>
       <c r="B10" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-GlobalTeleHost Corp.
+        <v xml:space="preserve">_x000d_
+GlobalTeleHost Corp._x000d_
 </v>
       </c>
       <c r="C10" t="str">
@@ -860,8 +571,8 @@
         <v>38.143.66.142</v>
       </c>
       <c r="B11" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-GlobalTeleHost Corp.
+        <v xml:space="preserve">_x000d_
+GlobalTeleHost Corp._x000d_
 </v>
       </c>
       <c r="C11" t="str">
@@ -876,8 +587,8 @@
         <v>108.156.60.17</v>
       </c>
       <c r="B12" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-Amazon.com Inc.
+        <v xml:space="preserve">_x000d_
+Amazon.com Inc._x000d_
 </v>
       </c>
       <c r="C12" t="str">
@@ -892,8 +603,8 @@
         <v>38.143.66.142</v>
       </c>
       <c r="B13" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-GlobalTeleHost Corp.
+        <v xml:space="preserve">_x000d_
+GlobalTeleHost Corp._x000d_
 </v>
       </c>
       <c r="C13" t="str">
@@ -908,21 +619,437 @@
         <v>38.143.66.142</v>
       </c>
       <c r="B14" t="str" xml:space="preserve">
+        <v xml:space="preserve">_x000d_
+GlobalTeleHost Corp._x000d_
+</v>
+      </c>
+      <c r="C14" t="str">
+        <v>NÃO CONSTA EM BLACK-LIST</v>
+      </c>
+      <c r="D14" t="str">
+        <v>https://www.abuseipdb.com/check/38.143.66.142</v>
+      </c>
+    </row>
+    <row r="15" xml:space="preserve">
+      <c r="A15" t="str">
+        <v>38.143.66.142</v>
+      </c>
+      <c r="B15" t="str" xml:space="preserve">
+        <v xml:space="preserve">_x000d_
+GlobalTeleHost Corp._x000d_
+</v>
+      </c>
+      <c r="C15" t="str">
+        <v>NÃO CONSTA EM BLACK-LIST</v>
+      </c>
+      <c r="D15" t="str">
+        <v>https://www.abuseipdb.com/check/38.143.66.142</v>
+      </c>
+    </row>
+    <row r="16" xml:space="preserve">
+      <c r="A16" t="str">
+        <v>38.143.66.142</v>
+      </c>
+      <c r="B16" t="str" xml:space="preserve">
+        <v xml:space="preserve">_x000d_
+GlobalTeleHost Corp._x000d_
+</v>
+      </c>
+      <c r="C16" t="str">
+        <v>NÃO CONSTA EM BLACK-LIST</v>
+      </c>
+      <c r="D16" t="str">
+        <v>https://www.abuseipdb.com/check/38.143.66.142</v>
+      </c>
+    </row>
+    <row r="17" xml:space="preserve">
+      <c r="A17" t="str">
+        <v>38.143.66.142</v>
+      </c>
+      <c r="B17" t="str" xml:space="preserve">
+        <v xml:space="preserve">_x000d_
+GlobalTeleHost Corp._x000d_
+</v>
+      </c>
+      <c r="C17" t="str">
+        <v>NÃO CONSTA EM BLACK-LIST</v>
+      </c>
+      <c r="D17" t="str">
+        <v>https://www.abuseipdb.com/check/38.143.66.142</v>
+      </c>
+    </row>
+    <row r="18" xml:space="preserve">
+      <c r="A18" t="str">
+        <v>38.143.66.142</v>
+      </c>
+      <c r="B18" t="str" xml:space="preserve">
+        <v xml:space="preserve">_x000d_
+GlobalTeleHost Corp._x000d_
+</v>
+      </c>
+      <c r="C18" t="str">
+        <v>NÃO CONSTA EM BLACK-LIST</v>
+      </c>
+      <c r="D18" t="str">
+        <v>https://www.abuseipdb.com/check/38.143.66.142</v>
+      </c>
+    </row>
+    <row r="19" xml:space="preserve">
+      <c r="A19" t="str">
+        <v>38.143.66.142</v>
+      </c>
+      <c r="B19" t="str" xml:space="preserve">
+        <v xml:space="preserve">_x000d_
+GlobalTeleHost Corp._x000d_
+</v>
+      </c>
+      <c r="C19" t="str">
+        <v>NÃO CONSTA EM BLACK-LIST</v>
+      </c>
+      <c r="D19" t="str">
+        <v>https://www.abuseipdb.com/check/38.143.66.142</v>
+      </c>
+    </row>
+    <row r="20" xml:space="preserve">
+      <c r="A20" t="str">
+        <v>38.143.66.142</v>
+      </c>
+      <c r="B20" t="str" xml:space="preserve">
+        <v xml:space="preserve">_x000d_
+GlobalTeleHost Corp._x000d_
+</v>
+      </c>
+      <c r="C20" t="str">
+        <v>NÃO CONSTA EM BLACK-LIST</v>
+      </c>
+      <c r="D20" t="str">
+        <v>https://www.abuseipdb.com/check/38.143.66.142</v>
+      </c>
+    </row>
+    <row r="21" xml:space="preserve">
+      <c r="A21" t="str">
+        <v>38.143.66.142</v>
+      </c>
+      <c r="B21" t="str" xml:space="preserve">
+        <v xml:space="preserve">_x000d_
+GlobalTeleHost Corp._x000d_
+</v>
+      </c>
+      <c r="C21" t="str">
+        <v>NÃO CONSTA EM BLACK-LIST</v>
+      </c>
+      <c r="D21" t="str">
+        <v>https://www.abuseipdb.com/check/38.143.66.142</v>
+      </c>
+    </row>
+    <row r="22" xml:space="preserve">
+      <c r="A22" t="str">
+        <v>38.143.66.142</v>
+      </c>
+      <c r="B22" t="str" xml:space="preserve">
+        <v xml:space="preserve">_x000d_
+GlobalTeleHost Corp._x000d_
+</v>
+      </c>
+      <c r="C22" t="str">
+        <v>NÃO CONSTA EM BLACK-LIST</v>
+      </c>
+      <c r="D22" t="str">
+        <v>https://www.abuseipdb.com/check/38.143.66.142</v>
+      </c>
+    </row>
+    <row r="23" xml:space="preserve">
+      <c r="A23" t="str">
+        <v>38.143.66.142</v>
+      </c>
+      <c r="B23" t="str" xml:space="preserve">
+        <v xml:space="preserve">_x000d_
+GlobalTeleHost Corp._x000d_
+</v>
+      </c>
+      <c r="C23" t="str">
+        <v>NÃO CONSTA EM BLACK-LIST</v>
+      </c>
+      <c r="D23" t="str">
+        <v>https://www.abuseipdb.com/check/38.143.66.142</v>
+      </c>
+    </row>
+    <row r="24" xml:space="preserve">
+      <c r="A24" t="str">
+        <v>38.143.66.142</v>
+      </c>
+      <c r="B24" t="str" xml:space="preserve">
+        <v xml:space="preserve">_x000d_
+GlobalTeleHost Corp._x000d_
+</v>
+      </c>
+      <c r="C24" t="str">
+        <v>NÃO CONSTA EM BLACK-LIST</v>
+      </c>
+      <c r="D24" t="str">
+        <v>https://www.abuseipdb.com/check/38.143.66.142</v>
+      </c>
+    </row>
+    <row r="25" xml:space="preserve">
+      <c r="A25" t="str">
+        <v>38.143.66.142</v>
+      </c>
+      <c r="B25" t="str" xml:space="preserve">
+        <v xml:space="preserve">_x000d_
+GlobalTeleHost Corp._x000d_
+</v>
+      </c>
+      <c r="C25" t="str">
+        <v>NÃO CONSTA EM BLACK-LIST</v>
+      </c>
+      <c r="D25" t="str">
+        <v>https://www.abuseipdb.com/check/38.143.66.142</v>
+      </c>
+    </row>
+    <row r="26" xml:space="preserve">
+      <c r="A26" t="str">
+        <v>38.143.66.142</v>
+      </c>
+      <c r="B26" t="str" xml:space="preserve">
+        <v xml:space="preserve">_x000d_
+GlobalTeleHost Corp._x000d_
+</v>
+      </c>
+      <c r="C26" t="str">
+        <v>NÃO CONSTA EM BLACK-LIST</v>
+      </c>
+      <c r="D26" t="str">
+        <v>https://www.abuseipdb.com/check/38.143.66.142</v>
+      </c>
+    </row>
+    <row r="27" xml:space="preserve">
+      <c r="A27" t="str">
+        <v>38.143.66.142</v>
+      </c>
+      <c r="B27" t="str" xml:space="preserve">
+        <v xml:space="preserve">_x000d_
+GlobalTeleHost Corp._x000d_
+</v>
+      </c>
+      <c r="C27" t="str">
+        <v>NÃO CONSTA EM BLACK-LIST</v>
+      </c>
+      <c r="D27" t="str">
+        <v>https://www.abuseipdb.com/check/38.143.66.142</v>
+      </c>
+    </row>
+    <row r="28" xml:space="preserve">
+      <c r="A28" t="str">
+        <v>38.143.66.142</v>
+      </c>
+      <c r="B28" t="str" xml:space="preserve">
+        <v xml:space="preserve">_x000d_
+GlobalTeleHost Corp._x000d_
+</v>
+      </c>
+      <c r="C28" t="str">
+        <v>NÃO CONSTA EM BLACK-LIST</v>
+      </c>
+      <c r="D28" t="str">
+        <v>https://www.abuseipdb.com/check/38.143.66.142</v>
+      </c>
+    </row>
+    <row r="29" xml:space="preserve">
+      <c r="A29" t="str">
+        <v>38.143.66.142</v>
+      </c>
+      <c r="B29" t="str" xml:space="preserve">
+        <v xml:space="preserve">_x000d_
+GlobalTeleHost Corp._x000d_
+</v>
+      </c>
+      <c r="C29" t="str">
+        <v>NÃO CONSTA EM BLACK-LIST</v>
+      </c>
+      <c r="D29" t="str">
+        <v>https://www.abuseipdb.com/check/38.143.66.142</v>
+      </c>
+    </row>
+    <row r="30" xml:space="preserve">
+      <c r="A30" t="str">
+        <v>38.143.66.142</v>
+      </c>
+      <c r="B30" t="str" xml:space="preserve">
+        <v xml:space="preserve">_x000d_
+GlobalTeleHost Corp._x000d_
+</v>
+      </c>
+      <c r="C30" t="str">
+        <v>NÃO CONSTA EM BLACK-LIST</v>
+      </c>
+      <c r="D30" t="str">
+        <v>https://www.abuseipdb.com/check/38.143.66.142</v>
+      </c>
+    </row>
+    <row r="31" xml:space="preserve">
+      <c r="A31" t="str">
+        <v>38.143.66.142</v>
+      </c>
+      <c r="B31" t="str" xml:space="preserve">
+        <v xml:space="preserve">_x000d_
+GlobalTeleHost Corp._x000d_
+</v>
+      </c>
+      <c r="C31" t="str">
+        <v>NÃO CONSTA EM BLACK-LIST</v>
+      </c>
+      <c r="D31" t="str">
+        <v>https://www.abuseipdb.com/check/38.143.66.142</v>
+      </c>
+    </row>
+    <row r="32" xml:space="preserve">
+      <c r="A32" t="str">
+        <v>38.143.66.142</v>
+      </c>
+      <c r="B32" t="str" xml:space="preserve">
+        <v xml:space="preserve">_x000d_
+GlobalTeleHost Corp._x000d_
+</v>
+      </c>
+      <c r="C32" t="str">
+        <v>NÃO CONSTA EM BLACK-LIST</v>
+      </c>
+      <c r="D32" t="str">
+        <v>https://www.abuseipdb.com/check/38.143.66.142</v>
+      </c>
+    </row>
+    <row r="33" xml:space="preserve">
+      <c r="A33" t="str">
+        <v>38.143.66.142</v>
+      </c>
+      <c r="B33" t="str" xml:space="preserve">
+        <v xml:space="preserve">_x000d_
+GlobalTeleHost Corp._x000d_
+</v>
+      </c>
+      <c r="C33" t="str">
+        <v>NÃO CONSTA EM BLACK-LIST</v>
+      </c>
+      <c r="D33" t="str">
+        <v>https://www.abuseipdb.com/check/38.143.66.142</v>
+      </c>
+    </row>
+    <row r="34" xml:space="preserve">
+      <c r="A34" t="str">
+        <v>38.143.66.142</v>
+      </c>
+      <c r="B34" t="str" xml:space="preserve">
         <v xml:space="preserve">
 GlobalTeleHost Corp.
 </v>
       </c>
-      <c r="C14" t="str">
+      <c r="C34" t="str">
         <v>NÃO CONSTA EM BLACK-LIST</v>
       </c>
-      <c r="D14" t="str">
+      <c r="D34" t="str">
+        <v>https://www.abuseipdb.com/check/38.143.66.142</v>
+      </c>
+    </row>
+    <row r="35" xml:space="preserve">
+      <c r="A35" t="str">
+        <v>38.143.66.142</v>
+      </c>
+      <c r="B35" t="str" xml:space="preserve">
+        <v xml:space="preserve">
+GlobalTeleHost Corp.
+</v>
+      </c>
+      <c r="C35" t="str">
+        <v>NÃO CONSTA EM BLACK-LIST</v>
+      </c>
+      <c r="D35" t="str">
+        <v>https://www.abuseipdb.com/check/38.143.66.142</v>
+      </c>
+    </row>
+    <row r="36" xml:space="preserve">
+      <c r="A36" t="str">
+        <v>38.143.66.142</v>
+      </c>
+      <c r="B36" t="str" xml:space="preserve">
+        <v xml:space="preserve">
+GlobalTeleHost Corp.
+</v>
+      </c>
+      <c r="C36" t="str">
+        <v>NÃO CONSTA EM BLACK-LIST</v>
+      </c>
+      <c r="D36" t="str">
+        <v>https://www.abuseipdb.com/check/38.143.66.142</v>
+      </c>
+    </row>
+    <row r="37" xml:space="preserve">
+      <c r="A37" t="str">
+        <v>38.143.66.142</v>
+      </c>
+      <c r="B37" t="str" xml:space="preserve">
+        <v xml:space="preserve">
+GlobalTeleHost Corp.
+</v>
+      </c>
+      <c r="C37" t="str">
+        <v>NÃO CONSTA EM BLACK-LIST</v>
+      </c>
+      <c r="D37" t="str">
+        <v>https://www.abuseipdb.com/check/38.143.66.142</v>
+      </c>
+    </row>
+    <row r="38" xml:space="preserve">
+      <c r="A38" t="str">
+        <v>38.143.66.142</v>
+      </c>
+      <c r="B38" t="str" xml:space="preserve">
+        <v xml:space="preserve">
+GlobalTeleHost Corp.
+</v>
+      </c>
+      <c r="C38" t="str">
+        <v>NÃO CONSTA EM BLACK-LIST</v>
+      </c>
+      <c r="D38" t="str">
+        <v>https://www.abuseipdb.com/check/38.143.66.142</v>
+      </c>
+    </row>
+    <row r="39" xml:space="preserve">
+      <c r="A39" t="str">
+        <v>38.143.66.142</v>
+      </c>
+      <c r="B39" t="str" xml:space="preserve">
+        <v xml:space="preserve">
+GlobalTeleHost Corp.
+</v>
+      </c>
+      <c r="C39" t="str">
+        <v>NÃO CONSTA EM BLACK-LIST</v>
+      </c>
+      <c r="D39" t="str">
+        <v>https://www.abuseipdb.com/check/38.143.66.142</v>
+      </c>
+    </row>
+    <row r="40" xml:space="preserve">
+      <c r="A40" t="str">
+        <v>38.143.66.142</v>
+      </c>
+      <c r="B40" t="str" xml:space="preserve">
+        <v xml:space="preserve">
+GlobalTeleHost Corp.
+</v>
+      </c>
+      <c r="C40" t="str">
+        <v>NÃO CONSTA EM BLACK-LIST</v>
+      </c>
+      <c r="D40" t="str">
         <v>https://www.abuseipdb.com/check/38.143.66.142</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:D14"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:D40"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -956,8 +1083,8 @@
         <v>46.29.10.30</v>
       </c>
       <c r="B2" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-Telemaks Ltd
+        <v xml:space="preserve">_x000d_
+Telemaks Ltd_x000d_
 </v>
       </c>
       <c r="C2" t="str">
@@ -975,8 +1102,8 @@
         <v>165.22.219.222</v>
       </c>
       <c r="B3" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-DigitalOcean LLC
+        <v xml:space="preserve">_x000d_
+DigitalOcean LLC_x000d_
 </v>
       </c>
       <c r="C3" t="str">
@@ -994,8 +1121,8 @@
         <v>185.81.68.21</v>
       </c>
       <c r="B4" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-Transcom LLC
+        <v xml:space="preserve">_x000d_
+Transcom LLC_x000d_
 </v>
       </c>
       <c r="C4" t="str">
@@ -1013,8 +1140,8 @@
         <v>114.139.46.250</v>
       </c>
       <c r="B5" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-China Telecom
+        <v xml:space="preserve">_x000d_
+China Telecom_x000d_
 </v>
       </c>
       <c r="C5" t="str">
@@ -1032,8 +1159,8 @@
         <v>51.195.47.176</v>
       </c>
       <c r="B6" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-OVH SAS
+        <v xml:space="preserve">_x000d_
+OVH SAS_x000d_
 </v>
       </c>
       <c r="C6" t="str">
@@ -1051,8 +1178,8 @@
         <v>161.97.160.249</v>
       </c>
       <c r="B7" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-Contabo GmbH
+        <v xml:space="preserve">_x000d_
+Contabo GmbH_x000d_
 </v>
       </c>
       <c r="C7" t="str">
@@ -1070,8 +1197,8 @@
         <v>192.24.192.231</v>
       </c>
       <c r="B8" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-Fuse Internet Access
+        <v xml:space="preserve">_x000d_
+Fuse Internet Access_x000d_
 </v>
       </c>
       <c r="C8" t="str">
@@ -1089,8 +1216,8 @@
         <v>49.232.218.12</v>
       </c>
       <c r="B9" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-Tencent Cloud Computing (Beijing) Co. Ltd.
+        <v xml:space="preserve">_x000d_
+Tencent Cloud Computing (Beijing) Co. Ltd._x000d_
 </v>
       </c>
       <c r="C9" t="str">
@@ -1108,8 +1235,8 @@
         <v>107.189.12.34</v>
       </c>
       <c r="B10" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-Frantech Solutions
+        <v xml:space="preserve">_x000d_
+Frantech Solutions_x000d_
 </v>
       </c>
       <c r="C10" t="str">
@@ -1127,8 +1254,8 @@
         <v>185.200.118.90</v>
       </c>
       <c r="B11" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-M247 Europe SRL
+        <v xml:space="preserve">_x000d_
+M247 Europe SRL_x000d_
 </v>
       </c>
       <c r="C11" t="str">
@@ -1146,8 +1273,8 @@
         <v>185.54.230.73</v>
       </c>
       <c r="B12" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-Avast Slovakia s.r.o.
+        <v xml:space="preserve">_x000d_
+Avast Slovakia s.r.o._x000d_
 </v>
       </c>
       <c r="C12" t="str">
@@ -1165,8 +1292,8 @@
         <v>176.58.107.136</v>
       </c>
       <c r="B13" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-Linode LLC
+        <v xml:space="preserve">_x000d_
+Linode LLC_x000d_
 </v>
       </c>
       <c r="C13" t="str">
@@ -1184,8 +1311,8 @@
         <v>80.82.70.228</v>
       </c>
       <c r="B14" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-Incrediserve Ltd
+        <v xml:space="preserve">_x000d_
+Incrediserve Ltd_x000d_
 </v>
       </c>
       <c r="C14" t="str">
@@ -1203,8 +1330,8 @@
         <v>46.101.76.96</v>
       </c>
       <c r="B15" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-DigitalOcean LLC
+        <v xml:space="preserve">_x000d_
+DigitalOcean LLC_x000d_
 </v>
       </c>
       <c r="C15" t="str">
@@ -1222,8 +1349,8 @@
         <v>43.153.67.197</v>
       </c>
       <c r="B16" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-Tencent Cloud Computing (Beijing) Co. Ltd.
+        <v xml:space="preserve">_x000d_
+Tencent Cloud Computing (Beijing) Co. Ltd._x000d_
 </v>
       </c>
       <c r="C16" t="str">
@@ -1241,8 +1368,8 @@
         <v>202.4.117.45</v>
       </c>
       <c r="B17" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-Dhakacom Limited
+        <v xml:space="preserve">_x000d_
+Dhakacom Limited_x000d_
 </v>
       </c>
       <c r="C17" t="str">
@@ -1260,8 +1387,8 @@
         <v>188.166.75.56</v>
       </c>
       <c r="B18" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-DigitalOcean LLC
+        <v xml:space="preserve">_x000d_
+DigitalOcean LLC_x000d_
 </v>
       </c>
       <c r="C18" t="str">
@@ -1279,8 +1406,8 @@
         <v>185.122.204.39</v>
       </c>
       <c r="B19" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-Starcrecium Limited
+        <v xml:space="preserve">_x000d_
+Starcrecium Limited_x000d_
 </v>
       </c>
       <c r="C19" t="str">
@@ -1298,8 +1425,8 @@
         <v>103.119.144.59</v>
       </c>
       <c r="B20" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-PT Bali Towerindo Sentra TBK
+        <v xml:space="preserve">_x000d_
+PT Bali Towerindo Sentra TBK_x000d_
 </v>
       </c>
       <c r="C20" t="str">
@@ -1317,8 +1444,8 @@
         <v>192.241.216.62</v>
       </c>
       <c r="B21" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-DigitalOcean LLC
+        <v xml:space="preserve">_x000d_
+DigitalOcean LLC_x000d_
 </v>
       </c>
       <c r="C21" t="str">
@@ -1336,8 +1463,8 @@
         <v>158.255.7.157</v>
       </c>
       <c r="B22" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-LLC Server v arendy
+        <v xml:space="preserve">_x000d_
+LLC Server v arendy_x000d_
 </v>
       </c>
       <c r="C22" t="str">
@@ -1355,8 +1482,8 @@
         <v>45.61.186.4</v>
       </c>
       <c r="B23" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-Frantech Solutions
+        <v xml:space="preserve">_x000d_
+Frantech Solutions_x000d_
 </v>
       </c>
       <c r="C23" t="str">
@@ -1374,8 +1501,8 @@
         <v>206.189.25.255</v>
       </c>
       <c r="B24" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-DigitalOcean LLC
+        <v xml:space="preserve">_x000d_
+DigitalOcean LLC_x000d_
 </v>
       </c>
       <c r="C24" t="str">
@@ -1393,8 +1520,8 @@
         <v>200.73.130.31</v>
       </c>
       <c r="B25" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-Telecom Argentina S.A.
+        <v xml:space="preserve">_x000d_
+Telecom Argentina S.A._x000d_
 </v>
       </c>
       <c r="C25" t="str">
@@ -1412,8 +1539,8 @@
         <v>164.88.86.170</v>
       </c>
       <c r="B26" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-Argus Holdings (Pty) Ltd
+        <v xml:space="preserve">_x000d_
+Argus Holdings (Pty) Ltd_x000d_
 </v>
       </c>
       <c r="C26" t="str">
@@ -1431,8 +1558,8 @@
         <v>139.162.77.84</v>
       </c>
       <c r="B27" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-Linode LLC
+        <v xml:space="preserve">_x000d_
+Linode LLC_x000d_
 </v>
       </c>
       <c r="C27" t="str">
@@ -1450,8 +1577,8 @@
         <v>192.227.134.78</v>
       </c>
       <c r="B28" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-ColoCrossing
+        <v xml:space="preserve">_x000d_
+ColoCrossing_x000d_
 </v>
       </c>
       <c r="C28" t="str">
@@ -1469,8 +1596,8 @@
         <v>51.89.41.120</v>
       </c>
       <c r="B29" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-OVH SAS
+        <v xml:space="preserve">_x000d_
+OVH SAS_x000d_
 </v>
       </c>
       <c r="C29" t="str">
@@ -1488,8 +1615,8 @@
         <v>43.153.71.131</v>
       </c>
       <c r="B30" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-Tencent Cloud Computing (Beijing) Co. Ltd.
+        <v xml:space="preserve">_x000d_
+Tencent Cloud Computing (Beijing) Co. Ltd._x000d_
 </v>
       </c>
       <c r="C30" t="str">
@@ -1507,8 +1634,8 @@
         <v>95.154.29.197</v>
       </c>
       <c r="B31" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-Stofa A/S
+        <v xml:space="preserve">_x000d_
+Stofa A/S_x000d_
 </v>
       </c>
       <c r="C31" t="str">
@@ -1526,8 +1653,8 @@
         <v>192.241.213.58</v>
       </c>
       <c r="B32" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-DigitalOcean LLC
+        <v xml:space="preserve">_x000d_
+DigitalOcean LLC_x000d_
 </v>
       </c>
       <c r="C32" t="str">
@@ -1545,8 +1672,8 @@
         <v>175.24.124.152</v>
       </c>
       <c r="B33" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-Tencent Cloud Computing (Beijing) Co. Ltd.
+        <v xml:space="preserve">_x000d_
+Tencent Cloud Computing (Beijing) Co. Ltd._x000d_
 </v>
       </c>
       <c r="C33" t="str">
@@ -1564,8 +1691,8 @@
         <v>92.255.85.239</v>
       </c>
       <c r="B34" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-Chang Way Technologies Co. Limited
+        <v xml:space="preserve">_x000d_
+Chang Way Technologies Co. Limited_x000d_
 </v>
       </c>
       <c r="C34" t="str">
@@ -1583,8 +1710,8 @@
         <v>159.65.192.80</v>
       </c>
       <c r="B35" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-DigitalOcean LLC
+        <v xml:space="preserve">_x000d_
+DigitalOcean LLC_x000d_
 </v>
       </c>
       <c r="C35" t="str">
@@ -1602,8 +1729,8 @@
         <v>205.164.107.52</v>
       </c>
       <c r="B36" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-Delta R Seguranca E Servicos Ltda
+        <v xml:space="preserve">_x000d_
+Delta R Seguranca E Servicos Ltda_x000d_
 </v>
       </c>
       <c r="C36" t="str">
@@ -1621,8 +1748,8 @@
         <v>192.241.206.47</v>
       </c>
       <c r="B37" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-DigitalOcean LLC
+        <v xml:space="preserve">_x000d_
+DigitalOcean LLC_x000d_
 </v>
       </c>
       <c r="C37" t="str">
@@ -1640,8 +1767,8 @@
         <v>192.241.200.47</v>
       </c>
       <c r="B38" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-DigitalOcean LLC
+        <v xml:space="preserve">_x000d_
+DigitalOcean LLC_x000d_
 </v>
       </c>
       <c r="C38" t="str">
@@ -1659,8 +1786,8 @@
         <v>145.239.198.34</v>
       </c>
       <c r="B39" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-OVH SAS
+        <v xml:space="preserve">_x000d_
+OVH SAS_x000d_
 </v>
       </c>
       <c r="C39" t="str">
@@ -1678,8 +1805,8 @@
         <v>198.199.96.218</v>
       </c>
       <c r="B40" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-DigitalOcean LLC
+        <v xml:space="preserve">_x000d_
+DigitalOcean LLC_x000d_
 </v>
       </c>
       <c r="C40" t="str">
@@ -1697,8 +1824,8 @@
         <v>139.99.62.61</v>
       </c>
       <c r="B41" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-OVH Hosting Inc.
+        <v xml:space="preserve">_x000d_
+OVH Hosting Inc._x000d_
 </v>
       </c>
       <c r="C41" t="str">
@@ -1716,8 +1843,8 @@
         <v>159.65.51.33</v>
       </c>
       <c r="B42" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-DigitalOcean LLC
+        <v xml:space="preserve">_x000d_
+DigitalOcean LLC_x000d_
 </v>
       </c>
       <c r="C42" t="str">
@@ -1735,8 +1862,8 @@
         <v>192.241.209.7</v>
       </c>
       <c r="B43" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-DigitalOcean LLC
+        <v xml:space="preserve">_x000d_
+DigitalOcean LLC_x000d_
 </v>
       </c>
       <c r="C43" t="str">
@@ -1754,8 +1881,8 @@
         <v>137.184.10.101</v>
       </c>
       <c r="B44" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-DigitalOcean LLC
+        <v xml:space="preserve">_x000d_
+DigitalOcean LLC_x000d_
 </v>
       </c>
       <c r="C44" t="str">
@@ -1773,8 +1900,8 @@
         <v>45.95.55.230</v>
       </c>
       <c r="B45" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-Fly Hosting
+        <v xml:space="preserve">_x000d_
+Fly Hosting_x000d_
 </v>
       </c>
       <c r="C45" t="str">
@@ -1792,8 +1919,8 @@
         <v>185.200.116.90</v>
       </c>
       <c r="B46" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-M247 Europe SRL
+        <v xml:space="preserve">_x000d_
+M247 Europe SRL_x000d_
 </v>
       </c>
       <c r="C46" t="str">
@@ -1811,8 +1938,8 @@
         <v>46.29.10.30</v>
       </c>
       <c r="B47" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-Telemaks Ltd
+        <v xml:space="preserve">_x000d_
+Telemaks Ltd_x000d_
 </v>
       </c>
       <c r="C47" t="str">
@@ -1830,8 +1957,8 @@
         <v>165.22.219.222</v>
       </c>
       <c r="B48" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-DigitalOcean LLC
+        <v xml:space="preserve">_x000d_
+DigitalOcean LLC_x000d_
 </v>
       </c>
       <c r="C48" t="str">
@@ -1849,8 +1976,8 @@
         <v>185.81.68.21</v>
       </c>
       <c r="B49" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-Transcom LLC
+        <v xml:space="preserve">_x000d_
+Transcom LLC_x000d_
 </v>
       </c>
       <c r="C49" t="str">
@@ -1868,8 +1995,8 @@
         <v>114.139.46.250</v>
       </c>
       <c r="B50" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-China Telecom
+        <v xml:space="preserve">_x000d_
+China Telecom_x000d_
 </v>
       </c>
       <c r="C50" t="str">
@@ -1887,8 +2014,8 @@
         <v>51.195.47.176</v>
       </c>
       <c r="B51" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-OVH SAS
+        <v xml:space="preserve">_x000d_
+OVH SAS_x000d_
 </v>
       </c>
       <c r="C51" t="str">
@@ -1906,8 +2033,8 @@
         <v>161.97.160.249</v>
       </c>
       <c r="B52" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-Contabo GmbH
+        <v xml:space="preserve">_x000d_
+Contabo GmbH_x000d_
 </v>
       </c>
       <c r="C52" t="str">
@@ -1925,8 +2052,8 @@
         <v>192.24.192.231</v>
       </c>
       <c r="B53" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-Fuse Internet Access
+        <v xml:space="preserve">_x000d_
+Fuse Internet Access_x000d_
 </v>
       </c>
       <c r="C53" t="str">
@@ -1944,8 +2071,8 @@
         <v>49.232.218.12</v>
       </c>
       <c r="B54" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-Tencent Cloud Computing (Beijing) Co. Ltd.
+        <v xml:space="preserve">_x000d_
+Tencent Cloud Computing (Beijing) Co. Ltd._x000d_
 </v>
       </c>
       <c r="C54" t="str">
@@ -1963,8 +2090,8 @@
         <v>107.189.12.34</v>
       </c>
       <c r="B55" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-Frantech Solutions
+        <v xml:space="preserve">_x000d_
+Frantech Solutions_x000d_
 </v>
       </c>
       <c r="C55" t="str">
@@ -1982,8 +2109,8 @@
         <v>185.200.118.90</v>
       </c>
       <c r="B56" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-M247 Europe SRL
+        <v xml:space="preserve">_x000d_
+M247 Europe SRL_x000d_
 </v>
       </c>
       <c r="C56" t="str">
@@ -2001,8 +2128,8 @@
         <v>185.54.230.73</v>
       </c>
       <c r="B57" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-Avast Slovakia s.r.o.
+        <v xml:space="preserve">_x000d_
+Avast Slovakia s.r.o._x000d_
 </v>
       </c>
       <c r="C57" t="str">
@@ -2020,8 +2147,8 @@
         <v>176.58.107.136</v>
       </c>
       <c r="B58" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-Linode LLC
+        <v xml:space="preserve">_x000d_
+Linode LLC_x000d_
 </v>
       </c>
       <c r="C58" t="str">
@@ -2039,8 +2166,8 @@
         <v>80.82.70.228</v>
       </c>
       <c r="B59" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-Incrediserve Ltd
+        <v xml:space="preserve">_x000d_
+Incrediserve Ltd_x000d_
 </v>
       </c>
       <c r="C59" t="str">
@@ -2058,8 +2185,8 @@
         <v>46.101.76.96</v>
       </c>
       <c r="B60" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-DigitalOcean LLC
+        <v xml:space="preserve">_x000d_
+DigitalOcean LLC_x000d_
 </v>
       </c>
       <c r="C60" t="str">
@@ -2077,8 +2204,8 @@
         <v>43.153.67.197</v>
       </c>
       <c r="B61" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-Tencent Cloud Computing (Beijing) Co. Ltd.
+        <v xml:space="preserve">_x000d_
+Tencent Cloud Computing (Beijing) Co. Ltd._x000d_
 </v>
       </c>
       <c r="C61" t="str">
@@ -2096,8 +2223,8 @@
         <v>202.4.117.45</v>
       </c>
       <c r="B62" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-Dhakacom Limited
+        <v xml:space="preserve">_x000d_
+Dhakacom Limited_x000d_
 </v>
       </c>
       <c r="C62" t="str">
@@ -2115,8 +2242,8 @@
         <v>188.166.75.56</v>
       </c>
       <c r="B63" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-DigitalOcean LLC
+        <v xml:space="preserve">_x000d_
+DigitalOcean LLC_x000d_
 </v>
       </c>
       <c r="C63" t="str">
@@ -2134,8 +2261,8 @@
         <v>185.122.204.39</v>
       </c>
       <c r="B64" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-Starcrecium Limited
+        <v xml:space="preserve">_x000d_
+Starcrecium Limited_x000d_
 </v>
       </c>
       <c r="C64" t="str">
@@ -2153,8 +2280,8 @@
         <v>103.119.144.59</v>
       </c>
       <c r="B65" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-PT Bali Towerindo Sentra TBK
+        <v xml:space="preserve">_x000d_
+PT Bali Towerindo Sentra TBK_x000d_
 </v>
       </c>
       <c r="C65" t="str">
@@ -2172,8 +2299,8 @@
         <v>192.241.216.62</v>
       </c>
       <c r="B66" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-DigitalOcean LLC
+        <v xml:space="preserve">_x000d_
+DigitalOcean LLC_x000d_
 </v>
       </c>
       <c r="C66" t="str">
@@ -2191,8 +2318,8 @@
         <v>158.255.7.157</v>
       </c>
       <c r="B67" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-LLC Server v arendy
+        <v xml:space="preserve">_x000d_
+LLC Server v arendy_x000d_
 </v>
       </c>
       <c r="C67" t="str">
@@ -2210,8 +2337,8 @@
         <v>45.61.186.4</v>
       </c>
       <c r="B68" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-Frantech Solutions
+        <v xml:space="preserve">_x000d_
+Frantech Solutions_x000d_
 </v>
       </c>
       <c r="C68" t="str">
@@ -2229,8 +2356,8 @@
         <v>206.189.25.255</v>
       </c>
       <c r="B69" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-DigitalOcean LLC
+        <v xml:space="preserve">_x000d_
+DigitalOcean LLC_x000d_
 </v>
       </c>
       <c r="C69" t="str">
@@ -2248,8 +2375,8 @@
         <v>200.73.130.31</v>
       </c>
       <c r="B70" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-Telecom Argentina S.A.
+        <v xml:space="preserve">_x000d_
+Telecom Argentina S.A._x000d_
 </v>
       </c>
       <c r="C70" t="str">
@@ -2267,8 +2394,8 @@
         <v>164.88.86.170</v>
       </c>
       <c r="B71" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-Argus Holdings (Pty) Ltd
+        <v xml:space="preserve">_x000d_
+Argus Holdings (Pty) Ltd_x000d_
 </v>
       </c>
       <c r="C71" t="str">
@@ -2286,8 +2413,8 @@
         <v>139.162.77.84</v>
       </c>
       <c r="B72" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-Linode LLC
+        <v xml:space="preserve">_x000d_
+Linode LLC_x000d_
 </v>
       </c>
       <c r="C72" t="str">
@@ -2305,8 +2432,8 @@
         <v>192.227.134.78</v>
       </c>
       <c r="B73" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-ColoCrossing
+        <v xml:space="preserve">_x000d_
+ColoCrossing_x000d_
 </v>
       </c>
       <c r="C73" t="str">
@@ -2324,8 +2451,8 @@
         <v>51.89.41.120</v>
       </c>
       <c r="B74" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-OVH SAS
+        <v xml:space="preserve">_x000d_
+OVH SAS_x000d_
 </v>
       </c>
       <c r="C74" t="str">
@@ -2343,8 +2470,8 @@
         <v>43.153.71.131</v>
       </c>
       <c r="B75" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-Tencent Cloud Computing (Beijing) Co. Ltd.
+        <v xml:space="preserve">_x000d_
+Tencent Cloud Computing (Beijing) Co. Ltd._x000d_
 </v>
       </c>
       <c r="C75" t="str">
@@ -2362,8 +2489,8 @@
         <v>95.154.29.197</v>
       </c>
       <c r="B76" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-Stofa A/S
+        <v xml:space="preserve">_x000d_
+Stofa A/S_x000d_
 </v>
       </c>
       <c r="C76" t="str">
@@ -2381,8 +2508,8 @@
         <v>192.241.213.58</v>
       </c>
       <c r="B77" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-DigitalOcean LLC
+        <v xml:space="preserve">_x000d_
+DigitalOcean LLC_x000d_
 </v>
       </c>
       <c r="C77" t="str">
@@ -2400,8 +2527,8 @@
         <v>175.24.124.152</v>
       </c>
       <c r="B78" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-Tencent Cloud Computing (Beijing) Co. Ltd.
+        <v xml:space="preserve">_x000d_
+Tencent Cloud Computing (Beijing) Co. Ltd._x000d_
 </v>
       </c>
       <c r="C78" t="str">
@@ -2419,8 +2546,8 @@
         <v>92.255.85.239</v>
       </c>
       <c r="B79" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-Chang Way Technologies Co. Limited
+        <v xml:space="preserve">_x000d_
+Chang Way Technologies Co. Limited_x000d_
 </v>
       </c>
       <c r="C79" t="str">
@@ -2438,8 +2565,8 @@
         <v>159.65.192.80</v>
       </c>
       <c r="B80" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-DigitalOcean LLC
+        <v xml:space="preserve">_x000d_
+DigitalOcean LLC_x000d_
 </v>
       </c>
       <c r="C80" t="str">
@@ -2457,8 +2584,8 @@
         <v>205.164.107.52</v>
       </c>
       <c r="B81" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-Delta R Seguranca E Servicos Ltda
+        <v xml:space="preserve">_x000d_
+Delta R Seguranca E Servicos Ltda_x000d_
 </v>
       </c>
       <c r="C81" t="str">
@@ -2476,8 +2603,8 @@
         <v>192.241.206.47</v>
       </c>
       <c r="B82" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-DigitalOcean LLC
+        <v xml:space="preserve">_x000d_
+DigitalOcean LLC_x000d_
 </v>
       </c>
       <c r="C82" t="str">
@@ -2495,8 +2622,8 @@
         <v>192.241.200.47</v>
       </c>
       <c r="B83" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-DigitalOcean LLC
+        <v xml:space="preserve">_x000d_
+DigitalOcean LLC_x000d_
 </v>
       </c>
       <c r="C83" t="str">
@@ -2514,8 +2641,8 @@
         <v>145.239.198.34</v>
       </c>
       <c r="B84" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-OVH SAS
+        <v xml:space="preserve">_x000d_
+OVH SAS_x000d_
 </v>
       </c>
       <c r="C84" t="str">
@@ -2533,8 +2660,8 @@
         <v>198.199.96.218</v>
       </c>
       <c r="B85" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-DigitalOcean LLC
+        <v xml:space="preserve">_x000d_
+DigitalOcean LLC_x000d_
 </v>
       </c>
       <c r="C85" t="str">
@@ -2552,8 +2679,8 @@
         <v>139.99.62.61</v>
       </c>
       <c r="B86" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-OVH Hosting Inc.
+        <v xml:space="preserve">_x000d_
+OVH Hosting Inc._x000d_
 </v>
       </c>
       <c r="C86" t="str">
@@ -2571,8 +2698,8 @@
         <v>159.65.51.33</v>
       </c>
       <c r="B87" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-DigitalOcean LLC
+        <v xml:space="preserve">_x000d_
+DigitalOcean LLC_x000d_
 </v>
       </c>
       <c r="C87" t="str">
@@ -2590,8 +2717,8 @@
         <v>192.241.209.7</v>
       </c>
       <c r="B88" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-DigitalOcean LLC
+        <v xml:space="preserve">_x000d_
+DigitalOcean LLC_x000d_
 </v>
       </c>
       <c r="C88" t="str">
@@ -2609,8 +2736,8 @@
         <v>137.184.10.101</v>
       </c>
       <c r="B89" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-DigitalOcean LLC
+        <v xml:space="preserve">_x000d_
+DigitalOcean LLC_x000d_
 </v>
       </c>
       <c r="C89" t="str">
@@ -2628,8 +2755,8 @@
         <v>45.95.55.230</v>
       </c>
       <c r="B90" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-Fly Hosting
+        <v xml:space="preserve">_x000d_
+Fly Hosting_x000d_
 </v>
       </c>
       <c r="C90" t="str">
@@ -2647,8 +2774,8 @@
         <v>185.200.116.90</v>
       </c>
       <c r="B91" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-M247 Europe SRL
+        <v xml:space="preserve">_x000d_
+M247 Europe SRL_x000d_
 </v>
       </c>
       <c r="C91" t="str">
@@ -2666,8 +2793,8 @@
         <v>46.29.10.30</v>
       </c>
       <c r="B92" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-Telemaks Ltd
+        <v xml:space="preserve">_x000d_
+Telemaks Ltd_x000d_
 </v>
       </c>
       <c r="C92" t="str">
@@ -2685,8 +2812,8 @@
         <v>165.22.219.222</v>
       </c>
       <c r="B93" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-DigitalOcean LLC
+        <v xml:space="preserve">_x000d_
+DigitalOcean LLC_x000d_
 </v>
       </c>
       <c r="C93" t="str">
@@ -2704,8 +2831,8 @@
         <v>185.81.68.21</v>
       </c>
       <c r="B94" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-Transcom LLC
+        <v xml:space="preserve">_x000d_
+Transcom LLC_x000d_
 </v>
       </c>
       <c r="C94" t="str">
@@ -2723,8 +2850,8 @@
         <v>114.139.46.250</v>
       </c>
       <c r="B95" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-China Telecom
+        <v xml:space="preserve">_x000d_
+China Telecom_x000d_
 </v>
       </c>
       <c r="C95" t="str">
@@ -2742,8 +2869,8 @@
         <v>51.195.47.176</v>
       </c>
       <c r="B96" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-OVH SAS
+        <v xml:space="preserve">_x000d_
+OVH SAS_x000d_
 </v>
       </c>
       <c r="C96" t="str">
@@ -2761,8 +2888,8 @@
         <v>161.97.160.249</v>
       </c>
       <c r="B97" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-Contabo GmbH
+        <v xml:space="preserve">_x000d_
+Contabo GmbH_x000d_
 </v>
       </c>
       <c r="C97" t="str">
@@ -2780,8 +2907,8 @@
         <v>192.24.192.231</v>
       </c>
       <c r="B98" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-Fuse Internet Access
+        <v xml:space="preserve">_x000d_
+Fuse Internet Access_x000d_
 </v>
       </c>
       <c r="C98" t="str">
@@ -2799,8 +2926,8 @@
         <v>49.232.218.12</v>
       </c>
       <c r="B99" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-Tencent Cloud Computing (Beijing) Co. Ltd.
+        <v xml:space="preserve">_x000d_
+Tencent Cloud Computing (Beijing) Co. Ltd._x000d_
 </v>
       </c>
       <c r="C99" t="str">
@@ -2818,8 +2945,8 @@
         <v>107.189.12.34</v>
       </c>
       <c r="B100" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-Frantech Solutions
+        <v xml:space="preserve">_x000d_
+Frantech Solutions_x000d_
 </v>
       </c>
       <c r="C100" t="str">
@@ -2837,8 +2964,8 @@
         <v>185.200.118.90</v>
       </c>
       <c r="B101" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-M247 Europe SRL
+        <v xml:space="preserve">_x000d_
+M247 Europe SRL_x000d_
 </v>
       </c>
       <c r="C101" t="str">
@@ -2856,8 +2983,8 @@
         <v>185.54.230.73</v>
       </c>
       <c r="B102" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-Avast Slovakia s.r.o.
+        <v xml:space="preserve">_x000d_
+Avast Slovakia s.r.o._x000d_
 </v>
       </c>
       <c r="C102" t="str">
@@ -2875,8 +3002,8 @@
         <v>176.58.107.136</v>
       </c>
       <c r="B103" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-Linode LLC
+        <v xml:space="preserve">_x000d_
+Linode LLC_x000d_
 </v>
       </c>
       <c r="C103" t="str">
@@ -2894,8 +3021,8 @@
         <v>80.82.70.228</v>
       </c>
       <c r="B104" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-Incrediserve Ltd
+        <v xml:space="preserve">_x000d_
+Incrediserve Ltd_x000d_
 </v>
       </c>
       <c r="C104" t="str">
@@ -2913,8 +3040,8 @@
         <v>46.101.76.96</v>
       </c>
       <c r="B105" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-DigitalOcean LLC
+        <v xml:space="preserve">_x000d_
+DigitalOcean LLC_x000d_
 </v>
       </c>
       <c r="C105" t="str">
@@ -2932,8 +3059,8 @@
         <v>43.153.67.197</v>
       </c>
       <c r="B106" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-Tencent Cloud Computing (Beijing) Co. Ltd.
+        <v xml:space="preserve">_x000d_
+Tencent Cloud Computing (Beijing) Co. Ltd._x000d_
 </v>
       </c>
       <c r="C106" t="str">
@@ -2951,8 +3078,8 @@
         <v>202.4.117.45</v>
       </c>
       <c r="B107" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-Dhakacom Limited
+        <v xml:space="preserve">_x000d_
+Dhakacom Limited_x000d_
 </v>
       </c>
       <c r="C107" t="str">
@@ -2970,8 +3097,8 @@
         <v>188.166.75.56</v>
       </c>
       <c r="B108" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-DigitalOcean LLC
+        <v xml:space="preserve">_x000d_
+DigitalOcean LLC_x000d_
 </v>
       </c>
       <c r="C108" t="str">
@@ -2989,8 +3116,8 @@
         <v>185.122.204.39</v>
       </c>
       <c r="B109" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-Starcrecium Limited
+        <v xml:space="preserve">_x000d_
+Starcrecium Limited_x000d_
 </v>
       </c>
       <c r="C109" t="str">
@@ -3008,8 +3135,8 @@
         <v>103.119.144.59</v>
       </c>
       <c r="B110" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-PT Bali Towerindo Sentra TBK
+        <v xml:space="preserve">_x000d_
+PT Bali Towerindo Sentra TBK_x000d_
 </v>
       </c>
       <c r="C110" t="str">
@@ -3027,8 +3154,8 @@
         <v>192.241.216.62</v>
       </c>
       <c r="B111" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-DigitalOcean LLC
+        <v xml:space="preserve">_x000d_
+DigitalOcean LLC_x000d_
 </v>
       </c>
       <c r="C111" t="str">
@@ -3046,8 +3173,8 @@
         <v>158.255.7.157</v>
       </c>
       <c r="B112" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-LLC Server v arendy
+        <v xml:space="preserve">_x000d_
+LLC Server v arendy_x000d_
 </v>
       </c>
       <c r="C112" t="str">
@@ -3065,8 +3192,8 @@
         <v>45.61.186.4</v>
       </c>
       <c r="B113" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-Frantech Solutions
+        <v xml:space="preserve">_x000d_
+Frantech Solutions_x000d_
 </v>
       </c>
       <c r="C113" t="str">
@@ -3084,8 +3211,8 @@
         <v>206.189.25.255</v>
       </c>
       <c r="B114" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-DigitalOcean LLC
+        <v xml:space="preserve">_x000d_
+DigitalOcean LLC_x000d_
 </v>
       </c>
       <c r="C114" t="str">
@@ -3103,8 +3230,8 @@
         <v>200.73.130.31</v>
       </c>
       <c r="B115" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-Telecom Argentina S.A.
+        <v xml:space="preserve">_x000d_
+Telecom Argentina S.A._x000d_
 </v>
       </c>
       <c r="C115" t="str">
@@ -3122,8 +3249,8 @@
         <v>164.88.86.170</v>
       </c>
       <c r="B116" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-Argus Holdings (Pty) Ltd
+        <v xml:space="preserve">_x000d_
+Argus Holdings (Pty) Ltd_x000d_
 </v>
       </c>
       <c r="C116" t="str">
@@ -3141,8 +3268,8 @@
         <v>139.162.77.84</v>
       </c>
       <c r="B117" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-Linode LLC
+        <v xml:space="preserve">_x000d_
+Linode LLC_x000d_
 </v>
       </c>
       <c r="C117" t="str">
@@ -3160,8 +3287,8 @@
         <v>192.227.134.78</v>
       </c>
       <c r="B118" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-ColoCrossing
+        <v xml:space="preserve">_x000d_
+ColoCrossing_x000d_
 </v>
       </c>
       <c r="C118" t="str">
@@ -3179,8 +3306,8 @@
         <v>51.89.41.120</v>
       </c>
       <c r="B119" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-OVH SAS
+        <v xml:space="preserve">_x000d_
+OVH SAS_x000d_
 </v>
       </c>
       <c r="C119" t="str">
@@ -3198,8 +3325,8 @@
         <v>43.153.71.131</v>
       </c>
       <c r="B120" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-Tencent Cloud Computing (Beijing) Co. Ltd.
+        <v xml:space="preserve">_x000d_
+Tencent Cloud Computing (Beijing) Co. Ltd._x000d_
 </v>
       </c>
       <c r="C120" t="str">
@@ -3217,8 +3344,8 @@
         <v>95.154.29.197</v>
       </c>
       <c r="B121" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-Stofa A/S
+        <v xml:space="preserve">_x000d_
+Stofa A/S_x000d_
 </v>
       </c>
       <c r="C121" t="str">
@@ -3236,8 +3363,8 @@
         <v>192.241.213.58</v>
       </c>
       <c r="B122" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-DigitalOcean LLC
+        <v xml:space="preserve">_x000d_
+DigitalOcean LLC_x000d_
 </v>
       </c>
       <c r="C122" t="str">
@@ -3255,8 +3382,8 @@
         <v>175.24.124.152</v>
       </c>
       <c r="B123" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-Tencent Cloud Computing (Beijing) Co. Ltd.
+        <v xml:space="preserve">_x000d_
+Tencent Cloud Computing (Beijing) Co. Ltd._x000d_
 </v>
       </c>
       <c r="C123" t="str">
@@ -3274,8 +3401,8 @@
         <v>92.255.85.239</v>
       </c>
       <c r="B124" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-Chang Way Technologies Co. Limited
+        <v xml:space="preserve">_x000d_
+Chang Way Technologies Co. Limited_x000d_
 </v>
       </c>
       <c r="C124" t="str">
@@ -3293,8 +3420,8 @@
         <v>159.65.192.80</v>
       </c>
       <c r="B125" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-DigitalOcean LLC
+        <v xml:space="preserve">_x000d_
+DigitalOcean LLC_x000d_
 </v>
       </c>
       <c r="C125" t="str">
@@ -3312,8 +3439,8 @@
         <v>205.164.107.52</v>
       </c>
       <c r="B126" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-Delta R Seguranca E Servicos Ltda
+        <v xml:space="preserve">_x000d_
+Delta R Seguranca E Servicos Ltda_x000d_
 </v>
       </c>
       <c r="C126" t="str">
@@ -3331,8 +3458,8 @@
         <v>192.241.206.47</v>
       </c>
       <c r="B127" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-DigitalOcean LLC
+        <v xml:space="preserve">_x000d_
+DigitalOcean LLC_x000d_
 </v>
       </c>
       <c r="C127" t="str">
@@ -3350,8 +3477,8 @@
         <v>192.241.200.47</v>
       </c>
       <c r="B128" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-DigitalOcean LLC
+        <v xml:space="preserve">_x000d_
+DigitalOcean LLC_x000d_
 </v>
       </c>
       <c r="C128" t="str">
@@ -3369,8 +3496,8 @@
         <v>145.239.198.34</v>
       </c>
       <c r="B129" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-OVH SAS
+        <v xml:space="preserve">_x000d_
+OVH SAS_x000d_
 </v>
       </c>
       <c r="C129" t="str">
@@ -3388,8 +3515,8 @@
         <v>198.199.96.218</v>
       </c>
       <c r="B130" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-DigitalOcean LLC
+        <v xml:space="preserve">_x000d_
+DigitalOcean LLC_x000d_
 </v>
       </c>
       <c r="C130" t="str">
@@ -3407,8 +3534,8 @@
         <v>139.99.62.61</v>
       </c>
       <c r="B131" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-OVH Hosting Inc.
+        <v xml:space="preserve">_x000d_
+OVH Hosting Inc._x000d_
 </v>
       </c>
       <c r="C131" t="str">
@@ -3426,8 +3553,8 @@
         <v>159.65.51.33</v>
       </c>
       <c r="B132" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-DigitalOcean LLC
+        <v xml:space="preserve">_x000d_
+DigitalOcean LLC_x000d_
 </v>
       </c>
       <c r="C132" t="str">
@@ -3445,8 +3572,8 @@
         <v>192.241.209.7</v>
       </c>
       <c r="B133" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-DigitalOcean LLC
+        <v xml:space="preserve">_x000d_
+DigitalOcean LLC_x000d_
 </v>
       </c>
       <c r="C133" t="str">
@@ -3464,8 +3591,8 @@
         <v>137.184.10.101</v>
       </c>
       <c r="B134" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-DigitalOcean LLC
+        <v xml:space="preserve">_x000d_
+DigitalOcean LLC_x000d_
 </v>
       </c>
       <c r="C134" t="str">
@@ -3483,8 +3610,8 @@
         <v>45.95.55.230</v>
       </c>
       <c r="B135" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-Fly Hosting
+        <v xml:space="preserve">_x000d_
+Fly Hosting_x000d_
 </v>
       </c>
       <c r="C135" t="str">
@@ -3502,8 +3629,8 @@
         <v>185.200.116.90</v>
       </c>
       <c r="B136" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-M247 Europe SRL
+        <v xml:space="preserve">_x000d_
+M247 Europe SRL_x000d_
 </v>
       </c>
       <c r="C136" t="str">
@@ -3521,8 +3648,8 @@
         <v>46.29.10.30</v>
       </c>
       <c r="B137" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-Telemaks Ltd
+        <v xml:space="preserve">_x000d_
+Telemaks Ltd_x000d_
 </v>
       </c>
       <c r="C137" t="str">
@@ -3540,8 +3667,8 @@
         <v>165.22.219.222</v>
       </c>
       <c r="B138" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-DigitalOcean LLC
+        <v xml:space="preserve">_x000d_
+DigitalOcean LLC_x000d_
 </v>
       </c>
       <c r="C138" t="str">
@@ -3559,8 +3686,8 @@
         <v>185.81.68.21</v>
       </c>
       <c r="B139" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-Transcom LLC
+        <v xml:space="preserve">_x000d_
+Transcom LLC_x000d_
 </v>
       </c>
       <c r="C139" t="str">
@@ -3578,8 +3705,8 @@
         <v>114.139.46.250</v>
       </c>
       <c r="B140" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-China Telecom
+        <v xml:space="preserve">_x000d_
+China Telecom_x000d_
 </v>
       </c>
       <c r="C140" t="str">
@@ -3597,8 +3724,8 @@
         <v>46.29.10.30</v>
       </c>
       <c r="B141" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-Telemaks Ltd
+        <v xml:space="preserve">_x000d_
+Telemaks Ltd_x000d_
 </v>
       </c>
       <c r="C141" t="str">
@@ -3616,8 +3743,8 @@
         <v>165.22.219.222</v>
       </c>
       <c r="B142" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-DigitalOcean LLC
+        <v xml:space="preserve">_x000d_
+DigitalOcean LLC_x000d_
 </v>
       </c>
       <c r="C142" t="str">
@@ -3635,8 +3762,8 @@
         <v>185.81.68.21</v>
       </c>
       <c r="B143" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-Transcom LLC
+        <v xml:space="preserve">_x000d_
+Transcom LLC_x000d_
 </v>
       </c>
       <c r="C143" t="str">
@@ -3654,8 +3781,8 @@
         <v>114.139.46.250</v>
       </c>
       <c r="B144" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-China Telecom
+        <v xml:space="preserve">_x000d_
+China Telecom_x000d_
 </v>
       </c>
       <c r="C144" t="str">
@@ -3673,8 +3800,8 @@
         <v>51.195.47.176</v>
       </c>
       <c r="B145" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-OVH SAS
+        <v xml:space="preserve">_x000d_
+OVH SAS_x000d_
 </v>
       </c>
       <c r="C145" t="str">
@@ -3692,8 +3819,8 @@
         <v>161.97.160.249</v>
       </c>
       <c r="B146" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-Contabo GmbH
+        <v xml:space="preserve">_x000d_
+Contabo GmbH_x000d_
 </v>
       </c>
       <c r="C146" t="str">
@@ -3711,8 +3838,8 @@
         <v>192.24.192.231</v>
       </c>
       <c r="B147" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-Fuse Internet Access
+        <v xml:space="preserve">_x000d_
+Fuse Internet Access_x000d_
 </v>
       </c>
       <c r="C147" t="str">
@@ -3730,8 +3857,8 @@
         <v>49.232.218.12</v>
       </c>
       <c r="B148" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-Tencent Cloud Computing (Beijing) Co. Ltd.
+        <v xml:space="preserve">_x000d_
+Tencent Cloud Computing (Beijing) Co. Ltd._x000d_
 </v>
       </c>
       <c r="C148" t="str">
@@ -3749,8 +3876,8 @@
         <v>107.189.12.34</v>
       </c>
       <c r="B149" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-Frantech Solutions
+        <v xml:space="preserve">_x000d_
+Frantech Solutions_x000d_
 </v>
       </c>
       <c r="C149" t="str">
@@ -3768,8 +3895,8 @@
         <v>185.200.118.90</v>
       </c>
       <c r="B150" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-M247 Europe SRL
+        <v xml:space="preserve">_x000d_
+M247 Europe SRL_x000d_
 </v>
       </c>
       <c r="C150" t="str">
@@ -3787,8 +3914,8 @@
         <v>185.54.230.73</v>
       </c>
       <c r="B151" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-Avast Slovakia s.r.o.
+        <v xml:space="preserve">_x000d_
+Avast Slovakia s.r.o._x000d_
 </v>
       </c>
       <c r="C151" t="str">
@@ -3806,8 +3933,8 @@
         <v>176.58.107.136</v>
       </c>
       <c r="B152" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-Linode LLC
+        <v xml:space="preserve">_x000d_
+Linode LLC_x000d_
 </v>
       </c>
       <c r="C152" t="str">
@@ -3825,8 +3952,8 @@
         <v>46.29.10.30</v>
       </c>
       <c r="B153" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-Telemaks Ltd
+        <v xml:space="preserve">_x000d_
+Telemaks Ltd_x000d_
 </v>
       </c>
       <c r="C153" t="str">
@@ -3844,8 +3971,8 @@
         <v>165.22.219.222</v>
       </c>
       <c r="B154" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-DigitalOcean LLC
+        <v xml:space="preserve">_x000d_
+DigitalOcean LLC_x000d_
 </v>
       </c>
       <c r="C154" t="str">
@@ -3863,8 +3990,8 @@
         <v>185.81.68.21</v>
       </c>
       <c r="B155" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-Transcom LLC
+        <v xml:space="preserve">_x000d_
+Transcom LLC_x000d_
 </v>
       </c>
       <c r="C155" t="str">
@@ -3882,8 +4009,8 @@
         <v>114.139.46.250</v>
       </c>
       <c r="B156" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-China Telecom
+        <v xml:space="preserve">_x000d_
+China Telecom_x000d_
 </v>
       </c>
       <c r="C156" t="str">
@@ -3901,8 +4028,8 @@
         <v>51.195.47.176</v>
       </c>
       <c r="B157" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-OVH SAS
+        <v xml:space="preserve">_x000d_
+OVH SAS_x000d_
 </v>
       </c>
       <c r="C157" t="str">
@@ -3920,8 +4047,8 @@
         <v>161.97.160.249</v>
       </c>
       <c r="B158" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-Contabo GmbH
+        <v xml:space="preserve">_x000d_
+Contabo GmbH_x000d_
 </v>
       </c>
       <c r="C158" t="str">
@@ -3939,8 +4066,8 @@
         <v>192.24.192.231</v>
       </c>
       <c r="B159" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-Fuse Internet Access
+        <v xml:space="preserve">_x000d_
+Fuse Internet Access_x000d_
 </v>
       </c>
       <c r="C159" t="str">
@@ -3958,8 +4085,8 @@
         <v>49.232.218.12</v>
       </c>
       <c r="B160" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-Tencent Cloud Computing (Beijing) Co. Ltd.
+        <v xml:space="preserve">_x000d_
+Tencent Cloud Computing (Beijing) Co. Ltd._x000d_
 </v>
       </c>
       <c r="C160" t="str">
@@ -3977,8 +4104,8 @@
         <v>107.189.12.34</v>
       </c>
       <c r="B161" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-Frantech Solutions
+        <v xml:space="preserve">_x000d_
+Frantech Solutions_x000d_
 </v>
       </c>
       <c r="C161" t="str">
@@ -3996,8 +4123,8 @@
         <v>185.200.118.90</v>
       </c>
       <c r="B162" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-M247 Europe SRL
+        <v xml:space="preserve">_x000d_
+M247 Europe SRL_x000d_
 </v>
       </c>
       <c r="C162" t="str">
@@ -4015,8 +4142,8 @@
         <v>185.54.230.73</v>
       </c>
       <c r="B163" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-Avast Slovakia s.r.o.
+        <v xml:space="preserve">_x000d_
+Avast Slovakia s.r.o._x000d_
 </v>
       </c>
       <c r="C163" t="str">
@@ -4034,8 +4161,8 @@
         <v>176.58.107.136</v>
       </c>
       <c r="B164" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-Linode LLC
+        <v xml:space="preserve">_x000d_
+Linode LLC_x000d_
 </v>
       </c>
       <c r="C164" t="str">
@@ -4053,8 +4180,8 @@
         <v>80.82.70.228</v>
       </c>
       <c r="B165" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-Incrediserve Ltd
+        <v xml:space="preserve">_x000d_
+Incrediserve Ltd_x000d_
 </v>
       </c>
       <c r="C165" t="str">
@@ -4072,8 +4199,8 @@
         <v>46.101.76.96</v>
       </c>
       <c r="B166" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-DigitalOcean LLC
+        <v xml:space="preserve">_x000d_
+DigitalOcean LLC_x000d_
 </v>
       </c>
       <c r="C166" t="str">
@@ -4091,8 +4218,8 @@
         <v>43.153.67.197</v>
       </c>
       <c r="B167" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-Tencent Cloud Computing (Beijing) Co. Ltd.
+        <v xml:space="preserve">_x000d_
+Tencent Cloud Computing (Beijing) Co. Ltd._x000d_
 </v>
       </c>
       <c r="C167" t="str">
@@ -4110,8 +4237,8 @@
         <v>202.4.117.45</v>
       </c>
       <c r="B168" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-Dhakacom Limited
+        <v xml:space="preserve">_x000d_
+Dhakacom Limited_x000d_
 </v>
       </c>
       <c r="C168" t="str">
@@ -4129,8 +4256,8 @@
         <v>188.166.75.56</v>
       </c>
       <c r="B169" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-DigitalOcean LLC
+        <v xml:space="preserve">_x000d_
+DigitalOcean LLC_x000d_
 </v>
       </c>
       <c r="C169" t="str">
@@ -4148,8 +4275,8 @@
         <v>185.122.204.39</v>
       </c>
       <c r="B170" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-Starcrecium Limited
+        <v xml:space="preserve">_x000d_
+Starcrecium Limited_x000d_
 </v>
       </c>
       <c r="C170" t="str">
@@ -4167,8 +4294,8 @@
         <v>103.119.144.59</v>
       </c>
       <c r="B171" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-PT Bali Towerindo Sentra TBK
+        <v xml:space="preserve">_x000d_
+PT Bali Towerindo Sentra TBK_x000d_
 </v>
       </c>
       <c r="C171" t="str">
@@ -4186,8 +4313,8 @@
         <v>192.241.216.62</v>
       </c>
       <c r="B172" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-DigitalOcean LLC
+        <v xml:space="preserve">_x000d_
+DigitalOcean LLC_x000d_
 </v>
       </c>
       <c r="C172" t="str">
@@ -4205,8 +4332,8 @@
         <v>158.255.7.157</v>
       </c>
       <c r="B173" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-LLC Server v arendy
+        <v xml:space="preserve">_x000d_
+LLC Server v arendy_x000d_
 </v>
       </c>
       <c r="C173" t="str">
@@ -4224,8 +4351,8 @@
         <v>45.61.186.4</v>
       </c>
       <c r="B174" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-Frantech Solutions
+        <v xml:space="preserve">_x000d_
+Frantech Solutions_x000d_
 </v>
       </c>
       <c r="C174" t="str">
@@ -4243,8 +4370,8 @@
         <v>206.189.25.255</v>
       </c>
       <c r="B175" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-DigitalOcean LLC
+        <v xml:space="preserve">_x000d_
+DigitalOcean LLC_x000d_
 </v>
       </c>
       <c r="C175" t="str">
@@ -4262,8 +4389,8 @@
         <v>200.73.130.31</v>
       </c>
       <c r="B176" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-Telecom Argentina S.A.
+        <v xml:space="preserve">_x000d_
+Telecom Argentina S.A._x000d_
 </v>
       </c>
       <c r="C176" t="str">
@@ -4281,8 +4408,8 @@
         <v>164.88.86.170</v>
       </c>
       <c r="B177" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-Argus Holdings (Pty) Ltd
+        <v xml:space="preserve">_x000d_
+Argus Holdings (Pty) Ltd_x000d_
 </v>
       </c>
       <c r="C177" t="str">
@@ -4300,8 +4427,8 @@
         <v>139.162.77.84</v>
       </c>
       <c r="B178" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-Linode LLC
+        <v xml:space="preserve">_x000d_
+Linode LLC_x000d_
 </v>
       </c>
       <c r="C178" t="str">
@@ -4319,8 +4446,8 @@
         <v>192.227.134.78</v>
       </c>
       <c r="B179" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-ColoCrossing
+        <v xml:space="preserve">_x000d_
+ColoCrossing_x000d_
 </v>
       </c>
       <c r="C179" t="str">
@@ -4338,8 +4465,8 @@
         <v>51.89.41.120</v>
       </c>
       <c r="B180" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-OVH SAS
+        <v xml:space="preserve">_x000d_
+OVH SAS_x000d_
 </v>
       </c>
       <c r="C180" t="str">
@@ -4357,8 +4484,8 @@
         <v>43.153.71.131</v>
       </c>
       <c r="B181" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-Tencent Cloud Computing (Beijing) Co. Ltd.
+        <v xml:space="preserve">_x000d_
+Tencent Cloud Computing (Beijing) Co. Ltd._x000d_
 </v>
       </c>
       <c r="C181" t="str">
@@ -4376,8 +4503,8 @@
         <v>95.154.29.197</v>
       </c>
       <c r="B182" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-Stofa A/S
+        <v xml:space="preserve">_x000d_
+Stofa A/S_x000d_
 </v>
       </c>
       <c r="C182" t="str">
@@ -4395,8 +4522,8 @@
         <v>192.241.213.58</v>
       </c>
       <c r="B183" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-DigitalOcean LLC
+        <v xml:space="preserve">_x000d_
+DigitalOcean LLC_x000d_
 </v>
       </c>
       <c r="C183" t="str">
@@ -4414,8 +4541,8 @@
         <v>175.24.124.152</v>
       </c>
       <c r="B184" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-Tencent Cloud Computing (Beijing) Co. Ltd.
+        <v xml:space="preserve">_x000d_
+Tencent Cloud Computing (Beijing) Co. Ltd._x000d_
 </v>
       </c>
       <c r="C184" t="str">
@@ -4433,8 +4560,8 @@
         <v>92.255.85.239</v>
       </c>
       <c r="B185" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-Chang Way Technologies Co. Limited
+        <v xml:space="preserve">_x000d_
+Chang Way Technologies Co. Limited_x000d_
 </v>
       </c>
       <c r="C185" t="str">
@@ -4452,8 +4579,8 @@
         <v>159.65.192.80</v>
       </c>
       <c r="B186" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-DigitalOcean LLC
+        <v xml:space="preserve">_x000d_
+DigitalOcean LLC_x000d_
 </v>
       </c>
       <c r="C186" t="str">
@@ -4471,8 +4598,8 @@
         <v>205.164.107.52</v>
       </c>
       <c r="B187" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-Delta R Seguranca E Servicos Ltda
+        <v xml:space="preserve">_x000d_
+Delta R Seguranca E Servicos Ltda_x000d_
 </v>
       </c>
       <c r="C187" t="str">
@@ -4490,8 +4617,8 @@
         <v>192.241.206.47</v>
       </c>
       <c r="B188" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-DigitalOcean LLC
+        <v xml:space="preserve">_x000d_
+DigitalOcean LLC_x000d_
 </v>
       </c>
       <c r="C188" t="str">
@@ -4509,8 +4636,8 @@
         <v>192.241.200.47</v>
       </c>
       <c r="B189" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-DigitalOcean LLC
+        <v xml:space="preserve">_x000d_
+DigitalOcean LLC_x000d_
 </v>
       </c>
       <c r="C189" t="str">
@@ -4528,8 +4655,8 @@
         <v>145.239.198.34</v>
       </c>
       <c r="B190" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-OVH SAS
+        <v xml:space="preserve">_x000d_
+OVH SAS_x000d_
 </v>
       </c>
       <c r="C190" t="str">
@@ -4547,8 +4674,8 @@
         <v>198.199.96.218</v>
       </c>
       <c r="B191" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-DigitalOcean LLC
+        <v xml:space="preserve">_x000d_
+DigitalOcean LLC_x000d_
 </v>
       </c>
       <c r="C191" t="str">
@@ -4566,8 +4693,8 @@
         <v>139.99.62.61</v>
       </c>
       <c r="B192" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-OVH Hosting Inc.
+        <v xml:space="preserve">_x000d_
+OVH Hosting Inc._x000d_
 </v>
       </c>
       <c r="C192" t="str">
@@ -4585,8 +4712,8 @@
         <v>159.65.51.33</v>
       </c>
       <c r="B193" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-DigitalOcean LLC
+        <v xml:space="preserve">_x000d_
+DigitalOcean LLC_x000d_
 </v>
       </c>
       <c r="C193" t="str">
@@ -4604,8 +4731,8 @@
         <v>192.241.209.7</v>
       </c>
       <c r="B194" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-DigitalOcean LLC
+        <v xml:space="preserve">_x000d_
+DigitalOcean LLC_x000d_
 </v>
       </c>
       <c r="C194" t="str">
@@ -4623,8 +4750,8 @@
         <v>137.184.10.101</v>
       </c>
       <c r="B195" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-DigitalOcean LLC
+        <v xml:space="preserve">_x000d_
+DigitalOcean LLC_x000d_
 </v>
       </c>
       <c r="C195" t="str">
@@ -4642,8 +4769,8 @@
         <v>45.95.55.230</v>
       </c>
       <c r="B196" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-Fly Hosting
+        <v xml:space="preserve">_x000d_
+Fly Hosting_x000d_
 </v>
       </c>
       <c r="C196" t="str">
@@ -4661,8 +4788,8 @@
         <v>185.200.116.90</v>
       </c>
       <c r="B197" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-M247 Europe SRL
+        <v xml:space="preserve">_x000d_
+M247 Europe SRL_x000d_
 </v>
       </c>
       <c r="C197" t="str">
@@ -4680,8 +4807,8 @@
         <v>192241205251</v>
       </c>
       <c r="B198" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-Telemaks Ltd
+        <v xml:space="preserve">_x000d_
+Telemaks Ltd_x000d_
 </v>
       </c>
       <c r="C198" t="str">
@@ -4699,8 +4826,8 @@
         <v>46.29.10.30</v>
       </c>
       <c r="B199" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-Telemaks Ltd
+        <v xml:space="preserve">_x000d_
+Telemaks Ltd_x000d_
 </v>
       </c>
       <c r="C199" t="str">
@@ -4718,8 +4845,8 @@
         <v>165.22.219.222</v>
       </c>
       <c r="B200" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-DigitalOcean LLC
+        <v xml:space="preserve">_x000d_
+DigitalOcean LLC_x000d_
 </v>
       </c>
       <c r="C200" t="str">
@@ -4737,8 +4864,8 @@
         <v>185.81.68.21</v>
       </c>
       <c r="B201" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-Transcom LLC
+        <v xml:space="preserve">_x000d_
+Transcom LLC_x000d_
 </v>
       </c>
       <c r="C201" t="str">
@@ -4756,8 +4883,8 @@
         <v>114.139.46.250</v>
       </c>
       <c r="B202" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-China Telecom
+        <v xml:space="preserve">_x000d_
+China Telecom_x000d_
 </v>
       </c>
       <c r="C202" t="str">
@@ -4775,8 +4902,8 @@
         <v>51.195.47.176</v>
       </c>
       <c r="B203" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-OVH SAS
+        <v xml:space="preserve">_x000d_
+OVH SAS_x000d_
 </v>
       </c>
       <c r="C203" t="str">
@@ -4794,8 +4921,8 @@
         <v>161.97.160.249</v>
       </c>
       <c r="B204" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-Contabo GmbH
+        <v xml:space="preserve">_x000d_
+Contabo GmbH_x000d_
 </v>
       </c>
       <c r="C204" t="str">
@@ -4813,8 +4940,8 @@
         <v>192.24.192.231</v>
       </c>
       <c r="B205" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-Fuse Internet Access
+        <v xml:space="preserve">_x000d_
+Fuse Internet Access_x000d_
 </v>
       </c>
       <c r="C205" t="str">
@@ -4832,8 +4959,8 @@
         <v>49.232.218.12</v>
       </c>
       <c r="B206" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-Tencent Cloud Computing (Beijing) Co. Ltd.
+        <v xml:space="preserve">_x000d_
+Tencent Cloud Computing (Beijing) Co. Ltd._x000d_
 </v>
       </c>
       <c r="C206" t="str">
@@ -4851,8 +4978,8 @@
         <v>107.189.12.34</v>
       </c>
       <c r="B207" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-Frantech Solutions
+        <v xml:space="preserve">_x000d_
+Frantech Solutions_x000d_
 </v>
       </c>
       <c r="C207" t="str">
@@ -4870,8 +4997,8 @@
         <v>185.200.118.90</v>
       </c>
       <c r="B208" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-M247 Europe SRL
+        <v xml:space="preserve">_x000d_
+M247 Europe SRL_x000d_
 </v>
       </c>
       <c r="C208" t="str">
@@ -4889,8 +5016,8 @@
         <v>185.54.230.73</v>
       </c>
       <c r="B209" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-Avast Slovakia s.r.o.
+        <v xml:space="preserve">_x000d_
+Avast Slovakia s.r.o._x000d_
 </v>
       </c>
       <c r="C209" t="str">
@@ -4908,8 +5035,8 @@
         <v>176.58.107.136</v>
       </c>
       <c r="B210" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-Linode LLC
+        <v xml:space="preserve">_x000d_
+Linode LLC_x000d_
 </v>
       </c>
       <c r="C210" t="str">
@@ -4927,8 +5054,8 @@
         <v>80.82.70.228</v>
       </c>
       <c r="B211" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-Incrediserve Ltd
+        <v xml:space="preserve">_x000d_
+Incrediserve Ltd_x000d_
 </v>
       </c>
       <c r="C211" t="str">
@@ -4946,8 +5073,8 @@
         <v>46.101.76.96</v>
       </c>
       <c r="B212" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-DigitalOcean LLC
+        <v xml:space="preserve">_x000d_
+DigitalOcean LLC_x000d_
 </v>
       </c>
       <c r="C212" t="str">
@@ -4965,8 +5092,8 @@
         <v>43.153.67.197</v>
       </c>
       <c r="B213" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-Tencent Cloud Computing (Beijing) Co. Ltd.
+        <v xml:space="preserve">_x000d_
+Tencent Cloud Computing (Beijing) Co. Ltd._x000d_
 </v>
       </c>
       <c r="C213" t="str">
@@ -4984,8 +5111,8 @@
         <v>202.4.117.45</v>
       </c>
       <c r="B214" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-Dhakacom Limited
+        <v xml:space="preserve">_x000d_
+Dhakacom Limited_x000d_
 </v>
       </c>
       <c r="C214" t="str">
@@ -5003,8 +5130,8 @@
         <v>188.166.75.56</v>
       </c>
       <c r="B215" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-DigitalOcean LLC
+        <v xml:space="preserve">_x000d_
+DigitalOcean LLC_x000d_
 </v>
       </c>
       <c r="C215" t="str">
@@ -5022,8 +5149,8 @@
         <v>185.122.204.39</v>
       </c>
       <c r="B216" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-Starcrecium Limited
+        <v xml:space="preserve">_x000d_
+Starcrecium Limited_x000d_
 </v>
       </c>
       <c r="C216" t="str">
@@ -5041,8 +5168,8 @@
         <v>103.119.144.59</v>
       </c>
       <c r="B217" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-PT Bali Towerindo Sentra TBK
+        <v xml:space="preserve">_x000d_
+PT Bali Towerindo Sentra TBK_x000d_
 </v>
       </c>
       <c r="C217" t="str">
@@ -5060,8 +5187,8 @@
         <v>192.241.216.62</v>
       </c>
       <c r="B218" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-DigitalOcean LLC
+        <v xml:space="preserve">_x000d_
+DigitalOcean LLC_x000d_
 </v>
       </c>
       <c r="C218" t="str">
@@ -5079,8 +5206,8 @@
         <v>158.255.7.157</v>
       </c>
       <c r="B219" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-LLC Server v arendy
+        <v xml:space="preserve">_x000d_
+LLC Server v arendy_x000d_
 </v>
       </c>
       <c r="C219" t="str">
@@ -5098,8 +5225,8 @@
         <v>45.61.186.4</v>
       </c>
       <c r="B220" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-Frantech Solutions
+        <v xml:space="preserve">_x000d_
+Frantech Solutions_x000d_
 </v>
       </c>
       <c r="C220" t="str">
@@ -5117,8 +5244,8 @@
         <v>206.189.25.255</v>
       </c>
       <c r="B221" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-DigitalOcean LLC
+        <v xml:space="preserve">_x000d_
+DigitalOcean LLC_x000d_
 </v>
       </c>
       <c r="C221" t="str">
@@ -5136,8 +5263,8 @@
         <v>200.73.130.31</v>
       </c>
       <c r="B222" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-Telecom Argentina S.A.
+        <v xml:space="preserve">_x000d_
+Telecom Argentina S.A._x000d_
 </v>
       </c>
       <c r="C222" t="str">
@@ -5155,8 +5282,8 @@
         <v>164.88.86.170</v>
       </c>
       <c r="B223" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-Argus Holdings (Pty) Ltd
+        <v xml:space="preserve">_x000d_
+Argus Holdings (Pty) Ltd_x000d_
 </v>
       </c>
       <c r="C223" t="str">
@@ -5174,8 +5301,8 @@
         <v>139.162.77.84</v>
       </c>
       <c r="B224" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-Linode LLC
+        <v xml:space="preserve">_x000d_
+Linode LLC_x000d_
 </v>
       </c>
       <c r="C224" t="str">
@@ -5194,4 +5321,608 @@
     <ignoredError numberStoredAsText="1" sqref="A1:E224"/>
   </ignoredErrors>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:CT2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" rightToLeft="0"/>
+  </sheetViews>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>harmless</v>
+      </c>
+      <c r="B1" t="str">
+        <v>malicious</v>
+      </c>
+      <c r="C1" t="str">
+        <v>suspicious</v>
+      </c>
+      <c r="D1" t="str">
+        <v>undetected</v>
+      </c>
+      <c r="E1" t="str">
+        <v>timeout</v>
+      </c>
+      <c r="F1" t="str">
+        <v>CMC Threat Intelligence</v>
+      </c>
+      <c r="G1" t="str">
+        <v>Snort IP sample list</v>
+      </c>
+      <c r="H1" t="str">
+        <v>0xSI_f33d</v>
+      </c>
+      <c r="I1" t="str">
+        <v>Armis</v>
+      </c>
+      <c r="J1" t="str">
+        <v>ViriBack</v>
+      </c>
+      <c r="K1" t="str">
+        <v>Comodo Valkyrie Verdict</v>
+      </c>
+      <c r="L1" t="str">
+        <v>PhishLabs</v>
+      </c>
+      <c r="M1" t="str">
+        <v>K7AntiVirus</v>
+      </c>
+      <c r="N1" t="str">
+        <v>CINS Army</v>
+      </c>
+      <c r="O1" t="str">
+        <v>Quttera</v>
+      </c>
+      <c r="P1" t="str">
+        <v>OpenPhish</v>
+      </c>
+      <c r="Q1" t="str">
+        <v>VX Vault</v>
+      </c>
+      <c r="R1" t="str">
+        <v>Web Security Guard</v>
+      </c>
+      <c r="S1" t="str">
+        <v>Scantitan</v>
+      </c>
+      <c r="T1" t="str">
+        <v>AlienVault</v>
+      </c>
+      <c r="U1" t="str">
+        <v>Sophos</v>
+      </c>
+      <c r="V1" t="str">
+        <v>Phishtank</v>
+      </c>
+      <c r="W1" t="str">
+        <v>EonScope</v>
+      </c>
+      <c r="X1" t="str">
+        <v>Cyan</v>
+      </c>
+      <c r="Y1" t="str">
+        <v>Spam404</v>
+      </c>
+      <c r="Z1" t="str">
+        <v>SecureBrain</v>
+      </c>
+      <c r="AA1" t="str">
+        <v>Hoplite Industries</v>
+      </c>
+      <c r="AB1" t="str">
+        <v>AutoShun</v>
+      </c>
+      <c r="AC1" t="str">
+        <v>Fortinet</v>
+      </c>
+      <c r="AD1" t="str">
+        <v>alphaMountain.ai</v>
+      </c>
+      <c r="AE1" t="str">
+        <v>Lionic</v>
+      </c>
+      <c r="AF1" t="str">
+        <v>Cyble</v>
+      </c>
+      <c r="AG1" t="str">
+        <v>Seclookup</v>
+      </c>
+      <c r="AH1" t="str">
+        <v>Virusdie External Site Scan</v>
+      </c>
+      <c r="AI1" t="str">
+        <v>Google Safebrowsing</v>
+      </c>
+      <c r="AJ1" t="str">
+        <v>SafeToOpen</v>
+      </c>
+      <c r="AK1" t="str">
+        <v>ADMINUSLabs</v>
+      </c>
+      <c r="AL1" t="str">
+        <v>CyberCrime</v>
+      </c>
+      <c r="AM1" t="str">
+        <v>Juniper Networks</v>
+      </c>
+      <c r="AN1" t="str">
+        <v>Heimdal Security</v>
+      </c>
+      <c r="AO1" t="str">
+        <v>CRDF</v>
+      </c>
+      <c r="AP1" t="str">
+        <v>Trustwave</v>
+      </c>
+      <c r="AQ1" t="str">
+        <v>AICC (MONITORAPP)</v>
+      </c>
+      <c r="AR1" t="str">
+        <v>CyRadar</v>
+      </c>
+      <c r="AS1" t="str">
+        <v>Dr.Web</v>
+      </c>
+      <c r="AT1" t="str">
+        <v>Emsisoft</v>
+      </c>
+      <c r="AU1" t="str">
+        <v>Abusix</v>
+      </c>
+      <c r="AV1" t="str">
+        <v>Webroot</v>
+      </c>
+      <c r="AW1" t="str">
+        <v>Avira</v>
+      </c>
+      <c r="AX1" t="str">
+        <v>securolytics</v>
+      </c>
+      <c r="AY1" t="str">
+        <v>Antiy-AVL</v>
+      </c>
+      <c r="AZ1" t="str">
+        <v>Acronis</v>
+      </c>
+      <c r="BA1" t="str">
+        <v>Quick Heal</v>
+      </c>
+      <c r="BB1" t="str">
+        <v>URLQuery</v>
+      </c>
+      <c r="BC1" t="str">
+        <v>Viettel Threat Intelligence</v>
+      </c>
+      <c r="BD1" t="str">
+        <v>DNS8</v>
+      </c>
+      <c r="BE1" t="str">
+        <v>benkow.cc</v>
+      </c>
+      <c r="BF1" t="str">
+        <v>EmergingThreats</v>
+      </c>
+      <c r="BG1" t="str">
+        <v>Chong Lua Dao</v>
+      </c>
+      <c r="BH1" t="str">
+        <v>Yandex Safebrowsing</v>
+      </c>
+      <c r="BI1" t="str">
+        <v>MalwareDomainList</v>
+      </c>
+      <c r="BJ1" t="str">
+        <v>Lumu</v>
+      </c>
+      <c r="BK1" t="str">
+        <v>zvelo</v>
+      </c>
+      <c r="BL1" t="str">
+        <v>Kaspersky</v>
+      </c>
+      <c r="BM1" t="str">
+        <v>Segasec</v>
+      </c>
+      <c r="BN1" t="str">
+        <v>Sucuri SiteCheck</v>
+      </c>
+      <c r="BO1" t="str">
+        <v>desenmascara.me</v>
+      </c>
+      <c r="BP1" t="str">
+        <v>URLhaus</v>
+      </c>
+      <c r="BQ1" t="str">
+        <v>PREBYTES</v>
+      </c>
+      <c r="BR1" t="str">
+        <v>StopForumSpam</v>
+      </c>
+      <c r="BS1" t="str">
+        <v>Blueliv</v>
+      </c>
+      <c r="BT1" t="str">
+        <v>Netcraft</v>
+      </c>
+      <c r="BU1" t="str">
+        <v>ZeroCERT</v>
+      </c>
+      <c r="BV1" t="str">
+        <v>Phishing Database</v>
+      </c>
+      <c r="BW1" t="str">
+        <v>MalwarePatrol</v>
+      </c>
+      <c r="BX1" t="str">
+        <v>MalBeacon</v>
+      </c>
+      <c r="BY1" t="str">
+        <v>IPsum</v>
+      </c>
+      <c r="BZ1" t="str">
+        <v>Malwared</v>
+      </c>
+      <c r="CA1" t="str">
+        <v>BitDefender</v>
+      </c>
+      <c r="CB1" t="str">
+        <v>GreenSnow</v>
+      </c>
+      <c r="CC1" t="str">
+        <v>G-Data</v>
+      </c>
+      <c r="CD1" t="str">
+        <v>StopBadware</v>
+      </c>
+      <c r="CE1" t="str">
+        <v>SCUMWARE.org</v>
+      </c>
+      <c r="CF1" t="str">
+        <v>ESTsecurity</v>
+      </c>
+      <c r="CG1" t="str">
+        <v>malwares.com URL checker</v>
+      </c>
+      <c r="CH1" t="str">
+        <v>NotMining</v>
+      </c>
+      <c r="CI1" t="str">
+        <v>Forcepoint ThreatSeeker</v>
+      </c>
+      <c r="CJ1" t="str">
+        <v>Certego</v>
+      </c>
+      <c r="CK1" t="str">
+        <v>ESET</v>
+      </c>
+      <c r="CL1" t="str">
+        <v>Threatsourcing</v>
+      </c>
+      <c r="CM1" t="str">
+        <v>MalSilo</v>
+      </c>
+      <c r="CN1" t="str">
+        <v>Nucleon</v>
+      </c>
+      <c r="CO1" t="str">
+        <v>BADWARE.INFO</v>
+      </c>
+      <c r="CP1" t="str">
+        <v>ThreatHive</v>
+      </c>
+      <c r="CQ1" t="str">
+        <v>FraudScore</v>
+      </c>
+      <c r="CR1" t="str">
+        <v>Tencent</v>
+      </c>
+      <c r="CS1" t="str">
+        <v>Bfore.Ai PreCrime</v>
+      </c>
+      <c r="CT1" t="str">
+        <v>Baidu-International</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2">
+        <v>93</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="F2" t="str">
+        <v>clean</v>
+      </c>
+      <c r="G2" t="str">
+        <v>clean</v>
+      </c>
+      <c r="H2" t="str">
+        <v>clean</v>
+      </c>
+      <c r="I2" t="str">
+        <v>clean</v>
+      </c>
+      <c r="J2" t="str">
+        <v>clean</v>
+      </c>
+      <c r="K2" t="str">
+        <v>clean</v>
+      </c>
+      <c r="L2" t="str">
+        <v>clean</v>
+      </c>
+      <c r="M2" t="str">
+        <v>clean</v>
+      </c>
+      <c r="N2" t="str">
+        <v>clean</v>
+      </c>
+      <c r="O2" t="str">
+        <v>clean</v>
+      </c>
+      <c r="P2" t="str">
+        <v>clean</v>
+      </c>
+      <c r="Q2" t="str">
+        <v>clean</v>
+      </c>
+      <c r="R2" t="str">
+        <v>clean</v>
+      </c>
+      <c r="S2" t="str">
+        <v>clean</v>
+      </c>
+      <c r="T2" t="str">
+        <v>clean</v>
+      </c>
+      <c r="U2" t="str">
+        <v>clean</v>
+      </c>
+      <c r="V2" t="str">
+        <v>clean</v>
+      </c>
+      <c r="W2" t="str">
+        <v>clean</v>
+      </c>
+      <c r="X2" t="str">
+        <v>clean</v>
+      </c>
+      <c r="Y2" t="str">
+        <v>clean</v>
+      </c>
+      <c r="Z2" t="str">
+        <v>clean</v>
+      </c>
+      <c r="AA2" t="str">
+        <v>clean</v>
+      </c>
+      <c r="AB2" t="str">
+        <v>clean</v>
+      </c>
+      <c r="AC2" t="str">
+        <v>clean</v>
+      </c>
+      <c r="AD2" t="str">
+        <v>clean</v>
+      </c>
+      <c r="AE2" t="str">
+        <v>clean</v>
+      </c>
+      <c r="AF2" t="str">
+        <v>clean</v>
+      </c>
+      <c r="AG2" t="str">
+        <v>clean</v>
+      </c>
+      <c r="AH2" t="str">
+        <v>clean</v>
+      </c>
+      <c r="AI2" t="str">
+        <v>clean</v>
+      </c>
+      <c r="AJ2" t="str">
+        <v>clean</v>
+      </c>
+      <c r="AK2" t="str">
+        <v>clean</v>
+      </c>
+      <c r="AL2" t="str">
+        <v>clean</v>
+      </c>
+      <c r="AM2" t="str">
+        <v>clean</v>
+      </c>
+      <c r="AN2" t="str">
+        <v>clean</v>
+      </c>
+      <c r="AO2" t="str">
+        <v>clean</v>
+      </c>
+      <c r="AP2" t="str">
+        <v>clean</v>
+      </c>
+      <c r="AQ2" t="str">
+        <v>clean</v>
+      </c>
+      <c r="AR2" t="str">
+        <v>clean</v>
+      </c>
+      <c r="AS2" t="str">
+        <v>clean</v>
+      </c>
+      <c r="AT2" t="str">
+        <v>clean</v>
+      </c>
+      <c r="AU2" t="str">
+        <v>clean</v>
+      </c>
+      <c r="AV2" t="str">
+        <v>clean</v>
+      </c>
+      <c r="AW2" t="str">
+        <v>clean</v>
+      </c>
+      <c r="AX2" t="str">
+        <v>clean</v>
+      </c>
+      <c r="AY2" t="str">
+        <v>clean</v>
+      </c>
+      <c r="AZ2" t="str">
+        <v>clean</v>
+      </c>
+      <c r="BA2" t="str">
+        <v>clean</v>
+      </c>
+      <c r="BB2" t="str">
+        <v>clean</v>
+      </c>
+      <c r="BC2" t="str">
+        <v>clean</v>
+      </c>
+      <c r="BD2" t="str">
+        <v>clean</v>
+      </c>
+      <c r="BE2" t="str">
+        <v>clean</v>
+      </c>
+      <c r="BF2" t="str">
+        <v>clean</v>
+      </c>
+      <c r="BG2" t="str">
+        <v>clean</v>
+      </c>
+      <c r="BH2" t="str">
+        <v>clean</v>
+      </c>
+      <c r="BI2" t="str">
+        <v>clean</v>
+      </c>
+      <c r="BJ2" t="str">
+        <v>clean</v>
+      </c>
+      <c r="BK2" t="str">
+        <v>clean</v>
+      </c>
+      <c r="BL2" t="str">
+        <v>clean</v>
+      </c>
+      <c r="BM2" t="str">
+        <v>clean</v>
+      </c>
+      <c r="BN2" t="str">
+        <v>clean</v>
+      </c>
+      <c r="BO2" t="str">
+        <v>clean</v>
+      </c>
+      <c r="BP2" t="str">
+        <v>clean</v>
+      </c>
+      <c r="BQ2" t="str">
+        <v>clean</v>
+      </c>
+      <c r="BR2" t="str">
+        <v>clean</v>
+      </c>
+      <c r="BS2" t="str">
+        <v>clean</v>
+      </c>
+      <c r="BT2" t="str">
+        <v>clean</v>
+      </c>
+      <c r="BU2" t="str">
+        <v>clean</v>
+      </c>
+      <c r="BV2" t="str">
+        <v>clean</v>
+      </c>
+      <c r="BW2" t="str">
+        <v>clean</v>
+      </c>
+      <c r="BX2" t="str">
+        <v>clean</v>
+      </c>
+      <c r="BY2" t="str">
+        <v>clean</v>
+      </c>
+      <c r="BZ2" t="str">
+        <v>clean</v>
+      </c>
+      <c r="CA2" t="str">
+        <v>clean</v>
+      </c>
+      <c r="CB2" t="str">
+        <v>clean</v>
+      </c>
+      <c r="CC2" t="str">
+        <v>clean</v>
+      </c>
+      <c r="CD2" t="str">
+        <v>clean</v>
+      </c>
+      <c r="CE2" t="str">
+        <v>clean</v>
+      </c>
+      <c r="CF2" t="str">
+        <v>clean</v>
+      </c>
+      <c r="CG2" t="str">
+        <v>clean</v>
+      </c>
+      <c r="CH2" t="str">
+        <v>clean</v>
+      </c>
+      <c r="CI2" t="str">
+        <v>clean</v>
+      </c>
+      <c r="CJ2" t="str">
+        <v>clean</v>
+      </c>
+      <c r="CK2" t="str">
+        <v>clean</v>
+      </c>
+      <c r="CL2" t="str">
+        <v>clean</v>
+      </c>
+      <c r="CM2" t="str">
+        <v>clean</v>
+      </c>
+      <c r="CN2" t="str">
+        <v>clean</v>
+      </c>
+      <c r="CO2" t="str">
+        <v>clean</v>
+      </c>
+      <c r="CP2" t="str">
+        <v>clean</v>
+      </c>
+      <c r="CQ2" t="str">
+        <v>clean</v>
+      </c>
+      <c r="CR2" t="str">
+        <v>clean</v>
+      </c>
+      <c r="CS2" t="str">
+        <v>clean</v>
+      </c>
+      <c r="CT2" t="str">
+        <v>clean</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1:CT2"/>
+  </ignoredErrors>
+</worksheet>
 </file>
</xml_diff>